<commit_message>
updated by:Alpna date:02-02-2013 updated time sheet
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,78 @@
   </si>
   <si>
     <t>TimeSheet_v1</t>
+  </si>
+  <si>
+    <t>Sr no</t>
+  </si>
+  <si>
+    <t>Formal Meeting (with Sir)</t>
+  </si>
+  <si>
+    <t>Alpna</t>
+  </si>
+  <si>
+    <t>RollNo</t>
+  </si>
+  <si>
+    <t>MT2012013</t>
+  </si>
+  <si>
+    <t>MT2012069</t>
+  </si>
+  <si>
+    <t>Kumari Suhani</t>
+  </si>
+  <si>
+    <t>MT2012105</t>
+  </si>
+  <si>
+    <t>MT2012119</t>
+  </si>
+  <si>
+    <t>MT2012122</t>
+  </si>
+  <si>
+    <t>MT2012129</t>
+  </si>
+  <si>
+    <t>MT2012140</t>
+  </si>
+  <si>
+    <t>Priyasmita Ghosh</t>
+  </si>
+  <si>
+    <t>Ruchika Sharma</t>
+  </si>
+  <si>
+    <t>Sai Naga Sravani Peraka</t>
+  </si>
+  <si>
+    <t>Satya Deepthi Bhagi</t>
+  </si>
+  <si>
+    <t>Sruti Davis</t>
+  </si>
+  <si>
+    <t>Informal Meeting(among team)</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>UseCaseDesign-Give Discount to Product</t>
+  </si>
+  <si>
+    <t>UseCaseDesign-Search</t>
+  </si>
+  <si>
+    <t>UseCaseDesign-Make Payment</t>
+  </si>
+  <si>
+    <t>DataBase-Design</t>
+  </si>
+  <si>
+    <t>Formal Meeting (with TA)</t>
   </si>
 </sst>
 </file>
@@ -72,8 +144,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,34 +480,518 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41296</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
+        <v>41296</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>41296</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41296</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
+        <v>41296</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
+        <v>41296</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1">
+        <v>41296</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1">
+        <v>41297</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1">
+        <v>41298</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1">
+        <v>41299</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1">
+        <v>41300</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1">
+        <v>41301</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1">
+        <v>41302</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1">
+        <v>41303</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1">
+        <v>41304</v>
+      </c>
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1">
+        <v>41305</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1">
+        <v>41306</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1">
+        <v>41306</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1">
+        <v>41307</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="D35" s="1">
+        <v>41308</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="D36" s="1">
+        <v>41309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="D37" s="1">
+        <v>41310</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="D38" s="1">
+        <v>41311</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="D39" s="1">
+        <v>41312</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
By: B S Deepthi Date: Feb 02 2012
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="13200" windowHeight="2076" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13200" windowHeight="2070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -125,14 +124,98 @@
   </si>
   <si>
     <t>Formal Meeting(with TA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team member 2: </t>
+  </si>
+  <si>
+    <t>Requirements for Ebay</t>
+  </si>
+  <si>
+    <t>Going through Ebay site and looked at some of its features by creating an user
+account</t>
+  </si>
+  <si>
+    <t>Studied some literature about Ebay</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Preparing the document "Know your friend" along with Team mates</t>
+  </si>
+  <si>
+    <t>Understanding Requirements</t>
+  </si>
+  <si>
+    <t>Understanding Requirements and thought of some feasible usecases
+ by discussing with team members</t>
+  </si>
+  <si>
+    <t>Preparing Usecase diagrams</t>
+  </si>
+  <si>
+    <t>Preparing Interaction Stories</t>
+  </si>
+  <si>
+    <t>Preparing Flow of events</t>
+  </si>
+  <si>
+    <t>Preparing Test Transactions</t>
+  </si>
+  <si>
+    <t>Requirements for MiniProject</t>
+  </si>
+  <si>
+    <t>Understanding Requirements for Student Profile Project</t>
+  </si>
+  <si>
+    <t>Database Design for Miniproject</t>
+  </si>
+  <si>
+    <t>Brainstorming for Database tables according to requirements</t>
+  </si>
+  <si>
+    <t>SVN Repository Setup</t>
+  </si>
+  <si>
+    <t>Created the SVN repositories for both Ebay and StudentProfile and done the
+initial SVN commit by creating the dynamic web projects and basic folder structures</t>
+  </si>
+  <si>
+    <t>Finalizing the Database schema by discussing with Teammembers and mentor</t>
+  </si>
+  <si>
+    <t>Coding for MiniProject</t>
+  </si>
+  <si>
+    <t>Done with DB.java and RuntimeSeetings.java with all created tables and 
+committed the changes to SVN</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Time Spent(Hrs)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -160,11 +243,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,12 +557,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
-    <col min="4" max="4" width="42.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4">
@@ -496,20 +588,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="A53" sqref="A53:F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.21875" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -834,7 +926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" customFormat="1">
+    <row r="25" spans="1:6">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -855,7 +947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" customFormat="1">
+    <row r="26" spans="1:6">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -876,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" customFormat="1">
+    <row r="27" spans="1:6">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -897,7 +989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" customFormat="1">
+    <row r="28" spans="1:6">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -918,7 +1010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" customFormat="1">
+    <row r="29" spans="1:6">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -939,7 +1031,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" customFormat="1">
+    <row r="30" spans="1:6">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -960,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" customFormat="1">
+    <row r="31" spans="1:6">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -977,9 +1069,8 @@
       <c r="E31" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" customFormat="1">
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -996,9 +1087,8 @@
       <c r="E32" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" customFormat="1">
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1015,9 +1105,8 @@
       <c r="E33" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" customFormat="1">
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1034,9 +1123,8 @@
       <c r="E34" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" customFormat="1">
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1057,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" customFormat="1">
+    <row r="36" spans="1:6">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1078,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" customFormat="1">
+    <row r="37" spans="1:6">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1099,7 +1187,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" customFormat="1">
+    <row r="38" spans="1:6">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1120,7 +1208,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" customFormat="1">
+    <row r="39" spans="1:6">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1141,7 +1229,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" customFormat="1">
+    <row r="40" spans="1:6">
       <c r="A40" s="3">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1162,7 +1250,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" customFormat="1">
+    <row r="41" spans="1:6">
       <c r="A41" s="3">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1183,7 +1271,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" customFormat="1">
+    <row r="42" spans="1:6">
       <c r="A42" s="3">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1204,7 +1292,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" customFormat="1">
+    <row r="43" spans="1:6">
       <c r="A43" s="3">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1225,7 +1313,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="1:6" customFormat="1">
+    <row r="44" spans="1:6">
       <c r="A44" s="3">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1246,7 +1334,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" customFormat="1">
+    <row r="45" spans="1:6">
       <c r="A45" s="3">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1254,9 +1342,8 @@
       <c r="D45" s="1">
         <v>41308</v>
       </c>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" customFormat="1">
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="3">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1264,9 +1351,8 @@
       <c r="D46" s="1">
         <v>41309</v>
       </c>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" customFormat="1">
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="3">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1274,9 +1360,8 @@
       <c r="D47" s="1">
         <v>41310</v>
       </c>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" customFormat="1">
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="3">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1284,9 +1369,8 @@
       <c r="D48" s="1">
         <v>41311</v>
       </c>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" customFormat="1">
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="3">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1294,7 +1378,631 @@
       <c r="D49" s="1">
         <v>41312</v>
       </c>
-      <c r="F49" s="2"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="45">
+      <c r="A54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="1">
+        <v>40912</v>
+      </c>
+      <c r="D54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="1">
+        <v>40913</v>
+      </c>
+      <c r="D55" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" t="s">
+        <v>39</v>
+      </c>
+      <c r="F55" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="1">
+        <v>40914</v>
+      </c>
+      <c r="D56" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="1">
+        <v>40915</v>
+      </c>
+      <c r="D57" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" t="s">
+        <v>39</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="1">
+        <v>40916</v>
+      </c>
+      <c r="D58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" t="s">
+        <v>41</v>
+      </c>
+      <c r="F58" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="1">
+        <v>40917</v>
+      </c>
+      <c r="D59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="1">
+        <v>40918</v>
+      </c>
+      <c r="D60" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="1">
+        <v>40919</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" t="s">
+        <v>25</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="1">
+        <v>40920</v>
+      </c>
+      <c r="D62" t="s">
+        <v>37</v>
+      </c>
+      <c r="E62" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="1">
+        <v>40921</v>
+      </c>
+      <c r="D63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="1">
+        <v>40922</v>
+      </c>
+      <c r="D64" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" t="s">
+        <v>25</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="1">
+        <v>40923</v>
+      </c>
+      <c r="D65" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="1">
+        <v>40924</v>
+      </c>
+      <c r="D66" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="45">
+      <c r="A67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="1">
+        <v>40925</v>
+      </c>
+      <c r="D67" t="s">
+        <v>37</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="1">
+        <v>40926</v>
+      </c>
+      <c r="D68" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="1">
+        <v>40927</v>
+      </c>
+      <c r="D69" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="1">
+        <v>40928</v>
+      </c>
+      <c r="D70" t="s">
+        <v>25</v>
+      </c>
+      <c r="E70" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="1">
+        <v>40929</v>
+      </c>
+      <c r="D71" t="s">
+        <v>37</v>
+      </c>
+      <c r="E71" t="s">
+        <v>44</v>
+      </c>
+      <c r="F71" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="1">
+        <v>40930</v>
+      </c>
+      <c r="D72" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="1">
+        <v>40931</v>
+      </c>
+      <c r="D73" t="s">
+        <v>25</v>
+      </c>
+      <c r="E73" t="s">
+        <v>25</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="1">
+        <v>40932</v>
+      </c>
+      <c r="D74" t="s">
+        <v>37</v>
+      </c>
+      <c r="E74" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="1">
+        <v>40933</v>
+      </c>
+      <c r="D75" t="s">
+        <v>25</v>
+      </c>
+      <c r="E75" t="s">
+        <v>25</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="1">
+        <v>40934</v>
+      </c>
+      <c r="D76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E76" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" s="1">
+        <v>40935</v>
+      </c>
+      <c r="D77" t="s">
+        <v>37</v>
+      </c>
+      <c r="E77" t="s">
+        <v>46</v>
+      </c>
+      <c r="F77" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" s="1">
+        <v>40936</v>
+      </c>
+      <c r="D78" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" t="s">
+        <v>47</v>
+      </c>
+      <c r="F78" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="1">
+        <v>40937</v>
+      </c>
+      <c r="D79" t="s">
+        <v>48</v>
+      </c>
+      <c r="E79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" s="1">
+        <v>40938</v>
+      </c>
+      <c r="D80" t="s">
+        <v>50</v>
+      </c>
+      <c r="E80" t="s">
+        <v>51</v>
+      </c>
+      <c r="F80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="60">
+      <c r="A81" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" s="1">
+        <v>40939</v>
+      </c>
+      <c r="D81" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F81" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" s="1">
+        <v>40940</v>
+      </c>
+      <c r="D82" t="s">
+        <v>50</v>
+      </c>
+      <c r="E82" t="s">
+        <v>54</v>
+      </c>
+      <c r="F82" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="45">
+      <c r="A83" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="1">
+        <v>40941</v>
+      </c>
+      <c r="D83" t="s">
+        <v>55</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F83" s="2">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1308,7 +2016,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by sravani date:2/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Time Spent(Hrs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team member 7: </t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:F53"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1404,7 +1407,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="45">
+    <row r="54" spans="1:6" ht="30">
       <c r="A54" s="3" t="s">
         <v>22</v>
       </c>
@@ -1664,7 +1667,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="45">
+    <row r="67" spans="1:6" ht="30">
       <c r="A67" s="3" t="s">
         <v>22</v>
       </c>
@@ -1944,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="60">
+    <row r="81" spans="1:6" ht="45">
       <c r="A81" s="3" t="s">
         <v>22</v>
       </c>
@@ -1984,7 +1987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="45">
+    <row r="83" spans="1:6" ht="30">
       <c r="A83" s="3" t="s">
         <v>22</v>
       </c>
@@ -2001,6 +2004,631 @@
         <v>56</v>
       </c>
       <c r="F83" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="30">
+      <c r="A89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89" s="1">
+        <v>40912</v>
+      </c>
+      <c r="D89" t="s">
+        <v>37</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" t="s">
+        <v>16</v>
+      </c>
+      <c r="C90" s="1">
+        <v>40913</v>
+      </c>
+      <c r="D90" t="s">
+        <v>37</v>
+      </c>
+      <c r="E90" t="s">
+        <v>39</v>
+      </c>
+      <c r="F90" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91" s="1">
+        <v>40914</v>
+      </c>
+      <c r="D91" t="s">
+        <v>25</v>
+      </c>
+      <c r="E91" t="s">
+        <v>25</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="1">
+        <v>40915</v>
+      </c>
+      <c r="D92" t="s">
+        <v>37</v>
+      </c>
+      <c r="E92" t="s">
+        <v>39</v>
+      </c>
+      <c r="F92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" s="1">
+        <v>40916</v>
+      </c>
+      <c r="D93" t="s">
+        <v>37</v>
+      </c>
+      <c r="E93" t="s">
+        <v>41</v>
+      </c>
+      <c r="F93" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" s="1">
+        <v>40917</v>
+      </c>
+      <c r="D94" t="s">
+        <v>25</v>
+      </c>
+      <c r="E94" t="s">
+        <v>25</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="1">
+        <v>40918</v>
+      </c>
+      <c r="D95" t="s">
+        <v>25</v>
+      </c>
+      <c r="E95" t="s">
+        <v>25</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" s="1">
+        <v>40919</v>
+      </c>
+      <c r="D96" t="s">
+        <v>25</v>
+      </c>
+      <c r="E96" t="s">
+        <v>25</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="1">
+        <v>40920</v>
+      </c>
+      <c r="D97" t="s">
+        <v>37</v>
+      </c>
+      <c r="E97" t="s">
+        <v>42</v>
+      </c>
+      <c r="F97" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="1">
+        <v>40921</v>
+      </c>
+      <c r="D98" t="s">
+        <v>25</v>
+      </c>
+      <c r="E98" t="s">
+        <v>25</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="1">
+        <v>40922</v>
+      </c>
+      <c r="D99" t="s">
+        <v>25</v>
+      </c>
+      <c r="E99" t="s">
+        <v>25</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" t="s">
+        <v>16</v>
+      </c>
+      <c r="C100" s="1">
+        <v>40923</v>
+      </c>
+      <c r="D100" t="s">
+        <v>25</v>
+      </c>
+      <c r="E100" t="s">
+        <v>25</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>21</v>
+      </c>
+      <c r="B101" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101" s="1">
+        <v>40924</v>
+      </c>
+      <c r="D101" t="s">
+        <v>25</v>
+      </c>
+      <c r="E101" t="s">
+        <v>25</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="30">
+      <c r="A102" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" s="1">
+        <v>40925</v>
+      </c>
+      <c r="D102" t="s">
+        <v>37</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F102" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>21</v>
+      </c>
+      <c r="B103" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103" s="1">
+        <v>40926</v>
+      </c>
+      <c r="D103" t="s">
+        <v>25</v>
+      </c>
+      <c r="E103" t="s">
+        <v>25</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" t="s">
+        <v>21</v>
+      </c>
+      <c r="B104" t="s">
+        <v>16</v>
+      </c>
+      <c r="C104" s="1">
+        <v>40927</v>
+      </c>
+      <c r="D104" t="s">
+        <v>25</v>
+      </c>
+      <c r="E104" t="s">
+        <v>25</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" s="1">
+        <v>40928</v>
+      </c>
+      <c r="D105" t="s">
+        <v>25</v>
+      </c>
+      <c r="E105" t="s">
+        <v>25</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>21</v>
+      </c>
+      <c r="B106" t="s">
+        <v>16</v>
+      </c>
+      <c r="C106" s="1">
+        <v>40929</v>
+      </c>
+      <c r="D106" t="s">
+        <v>37</v>
+      </c>
+      <c r="E106" t="s">
+        <v>44</v>
+      </c>
+      <c r="F106" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
+        <v>21</v>
+      </c>
+      <c r="B107" t="s">
+        <v>16</v>
+      </c>
+      <c r="C107" s="1">
+        <v>40930</v>
+      </c>
+      <c r="D107" t="s">
+        <v>25</v>
+      </c>
+      <c r="E107" t="s">
+        <v>25</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" s="1">
+        <v>40931</v>
+      </c>
+      <c r="D108" t="s">
+        <v>25</v>
+      </c>
+      <c r="E108" t="s">
+        <v>25</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
+        <v>21</v>
+      </c>
+      <c r="B109" t="s">
+        <v>16</v>
+      </c>
+      <c r="C109" s="1">
+        <v>40932</v>
+      </c>
+      <c r="D109" t="s">
+        <v>37</v>
+      </c>
+      <c r="E109" t="s">
+        <v>45</v>
+      </c>
+      <c r="F109" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" t="s">
+        <v>21</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110" s="1">
+        <v>40933</v>
+      </c>
+      <c r="D110" t="s">
+        <v>25</v>
+      </c>
+      <c r="E110" t="s">
+        <v>25</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>21</v>
+      </c>
+      <c r="B111" t="s">
+        <v>16</v>
+      </c>
+      <c r="C111" s="1">
+        <v>40934</v>
+      </c>
+      <c r="D111" t="s">
+        <v>25</v>
+      </c>
+      <c r="E111" t="s">
+        <v>25</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112" t="s">
+        <v>16</v>
+      </c>
+      <c r="C112" s="1">
+        <v>40935</v>
+      </c>
+      <c r="D112" t="s">
+        <v>37</v>
+      </c>
+      <c r="E112" t="s">
+        <v>46</v>
+      </c>
+      <c r="F112" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" t="s">
+        <v>21</v>
+      </c>
+      <c r="B113" t="s">
+        <v>16</v>
+      </c>
+      <c r="C113" s="1">
+        <v>40936</v>
+      </c>
+      <c r="D113" t="s">
+        <v>37</v>
+      </c>
+      <c r="E113" t="s">
+        <v>47</v>
+      </c>
+      <c r="F113" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" t="s">
+        <v>21</v>
+      </c>
+      <c r="B114" t="s">
+        <v>16</v>
+      </c>
+      <c r="C114" s="1">
+        <v>40937</v>
+      </c>
+      <c r="D114" t="s">
+        <v>48</v>
+      </c>
+      <c r="E114" t="s">
+        <v>49</v>
+      </c>
+      <c r="F114" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" t="s">
+        <v>21</v>
+      </c>
+      <c r="B115" t="s">
+        <v>16</v>
+      </c>
+      <c r="C115" s="1">
+        <v>40938</v>
+      </c>
+      <c r="D115" t="s">
+        <v>50</v>
+      </c>
+      <c r="E115" t="s">
+        <v>51</v>
+      </c>
+      <c r="F115" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" t="s">
+        <v>21</v>
+      </c>
+      <c r="B116" t="s">
+        <v>16</v>
+      </c>
+      <c r="C116" s="1">
+        <v>41305</v>
+      </c>
+      <c r="D116" t="s">
+        <v>34</v>
+      </c>
+      <c r="E116" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F116" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" t="s">
+        <v>21</v>
+      </c>
+      <c r="B117" t="s">
+        <v>16</v>
+      </c>
+      <c r="C117" s="1">
+        <v>40940</v>
+      </c>
+      <c r="D117" t="s">
+        <v>50</v>
+      </c>
+      <c r="E117" t="s">
+        <v>54</v>
+      </c>
+      <c r="F117" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="45">
+      <c r="A118" t="s">
+        <v>21</v>
+      </c>
+      <c r="B118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C118" s="1">
+        <v>40941</v>
+      </c>
+      <c r="D118" t="s">
+        <v>52</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F118" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date: 03-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11970" windowHeight="3645" activeTab="5"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="13035" windowHeight="5790" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,8 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1:L12"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:M3"/>
 </workbook>
 </file>
 
@@ -279,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -332,6 +332,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1413,11 +1416,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="21" t="s">
@@ -1449,7 +1457,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="180">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
@@ -1709,7 +1717,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="225">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="20" t="s">
         <v>16</v>
       </c>
@@ -1989,8 +1997,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="345">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:6" ht="45">
+      <c r="A30" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="17" t="s">
@@ -2029,7 +2037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="225">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="20" t="s">
         <v>16</v>
       </c>
@@ -2051,6 +2059,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2838,7 +2847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -2849,7 +2858,7 @@
     <col min="6" max="16384" width="11.7109375" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="34" customFormat="1">
+    <row r="1" spans="1:7">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2869,7 +2878,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="34" customFormat="1">
+    <row r="2" spans="1:7">
       <c r="A2" s="21"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2877,7 +2886,7 @@
       <c r="E2" s="40"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:7" s="34" customFormat="1">
+    <row r="3" spans="1:7">
       <c r="A3" s="21"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -2885,7 +2894,7 @@
       <c r="E3" s="40"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:7" s="34" customFormat="1">
+    <row r="4" spans="1:7">
       <c r="A4" s="21"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -2893,7 +2902,7 @@
       <c r="E4" s="40"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:7" s="34" customFormat="1">
+    <row r="5" spans="1:7">
       <c r="A5" s="21"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -2901,7 +2910,7 @@
       <c r="E5" s="40"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:7" s="34" customFormat="1">
+    <row r="6" spans="1:7">
       <c r="A6" s="34" t="s">
         <v>61</v>
       </c>
@@ -2914,7 +2923,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" s="34" customFormat="1" ht="45">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="34" t="s">
         <v>61</v>
       </c>
@@ -2934,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="34" customFormat="1">
+    <row r="8" spans="1:7">
       <c r="A8" s="34" t="s">
         <v>61</v>
       </c>
@@ -2948,7 +2957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="34" customFormat="1" ht="45">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="34" t="s">
         <v>61</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="34" customFormat="1" ht="165">
+    <row r="10" spans="1:7" ht="75">
       <c r="A10" s="34" t="s">
         <v>61</v>
       </c>
@@ -2988,7 +2997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="34" customFormat="1" ht="75">
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="34" t="s">
         <v>61</v>
       </c>
@@ -3008,7 +3017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="34" customFormat="1" ht="60">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="34" t="s">
         <v>61</v>
       </c>
@@ -3025,7 +3034,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="34" customFormat="1" ht="45">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="34" t="s">
         <v>61</v>
       </c>
@@ -3045,7 +3054,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="34" customFormat="1">
+    <row r="14" spans="1:7">
       <c r="A14" s="34" t="s">
         <v>61</v>
       </c>
@@ -3059,7 +3068,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="34" customFormat="1" ht="45">
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="34" t="s">
         <v>61</v>
       </c>
@@ -3079,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="34" customFormat="1" ht="45">
+    <row r="16" spans="1:7">
       <c r="A16" s="34" t="s">
         <v>61</v>
       </c>
@@ -3099,7 +3108,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="34" customFormat="1" ht="75">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="34" t="s">
         <v>61</v>
       </c>
@@ -3119,7 +3128,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="34" customFormat="1" ht="45">
+    <row r="18" spans="1:6">
       <c r="A18" s="34" t="s">
         <v>61</v>
       </c>
@@ -3139,7 +3148,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="34" customFormat="1" ht="45">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="34" t="s">
         <v>61</v>
       </c>
@@ -3159,7 +3168,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="34" customFormat="1" ht="30">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="37" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
updated by:Alpna time:22:25 date:03-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="3645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="3645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>Done with login functionality by maintaining user session and also included the basic  layout using tiles.Committed the changes to SVN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team member 7: </t>
+  </si>
+  <si>
+    <t>Sai Naga Sravani Peraka</t>
+  </si>
+  <si>
+    <t>MT2012122</t>
   </si>
 </sst>
 </file>
@@ -284,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -339,6 +348,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F135"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119:F119"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1355,12 +1376,18 @@
       <c r="A120" s="16">
         <v>14</v>
       </c>
-      <c r="B120" s="13"/>
-      <c r="C120" s="13"/>
+      <c r="B120" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="42" t="s">
+        <v>11</v>
+      </c>
       <c r="D120" s="14">
         <v>41308</v>
       </c>
-      <c r="E120" s="13"/>
+      <c r="E120" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="F120" s="13"/>
     </row>
     <row r="121" spans="1:6">
@@ -1418,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -3239,12 +3266,650 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="44"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="180">
+      <c r="A3" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="43">
+        <v>40912</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="43">
+        <v>40913</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="43">
+        <v>40914</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="43">
+        <v>40915</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="43">
+        <v>40916</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="43">
+        <v>40917</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="43">
+        <v>40918</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="43">
+        <v>40919</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="43">
+        <v>40920</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="43">
+        <v>40921</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="43">
+        <v>40922</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="43">
+        <v>40923</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="43">
+        <v>40924</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="225">
+      <c r="A16" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="43">
+        <v>40925</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="43">
+        <v>40926</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="43">
+        <v>40927</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="43">
+        <v>40928</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="43">
+        <v>40929</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="43">
+        <v>40930</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="43">
+        <v>40931</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="43">
+        <v>40932</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="43">
+        <v>40933</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="43">
+        <v>40934</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="43">
+        <v>40935</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="43">
+        <v>40936</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="43">
+        <v>40937</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="43">
+        <v>40938</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="43">
+        <v>41305</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="F30" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="43">
+        <v>40940</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="345">
+      <c r="A32" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="43">
+        <v>40941</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="44">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated time sheet name-Alpna time-22:51 date-03-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="3645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="3645" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -691,10 +691,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F135"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F120" sqref="F120"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -707,49 +707,299 @@
     <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:4">
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="4:4">
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="4:4">
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="4:4">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="4:4">
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="4:4">
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="4:4">
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="4:4">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="4:4">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="4:4">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="4:4">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="4:4">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="4:4">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="4:4">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="4:4">
+    <row r="1" spans="1:6">
+      <c r="A1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="14">
+        <v>41296</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14">
+        <v>41297</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14">
+        <v>41298</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="14">
+        <v>41299</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="14">
+        <v>41300</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="14">
+        <v>41301</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="14">
+        <v>41302</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="16">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="14">
+        <v>41303</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="16">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="14">
+        <v>41304</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="16">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="14">
+        <v>41305</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="16">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="14">
+        <v>41306</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="16">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="14">
+        <v>41306</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="16">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="14">
+        <v>41307</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="16">
+        <v>14</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="14">
+        <v>41308</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="4:4">
@@ -1098,320 +1348,28 @@
       <c r="C105" s="1"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="106" spans="1:6">
-      <c r="A106" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B106" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C106" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D106" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E106" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F106" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="16">
-        <v>1</v>
-      </c>
-      <c r="B107" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D107" s="14">
-        <v>41296</v>
-      </c>
-      <c r="E107" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F107" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108" s="16">
-        <v>2</v>
-      </c>
-      <c r="B108" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C108" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" s="14">
-        <v>41297</v>
-      </c>
-      <c r="E108" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F108" s="13"/>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109" s="16">
-        <v>3</v>
-      </c>
-      <c r="B109" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D109" s="14">
-        <v>41298</v>
-      </c>
-      <c r="E109" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F109" s="15">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110" s="16">
-        <v>4</v>
-      </c>
-      <c r="B110" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C110" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D110" s="14">
-        <v>41299</v>
-      </c>
-      <c r="E110" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F110" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" s="16">
-        <v>5</v>
-      </c>
-      <c r="B111" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C111" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D111" s="14">
-        <v>41300</v>
-      </c>
-      <c r="E111" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F111" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112" s="16">
-        <v>6</v>
-      </c>
-      <c r="B112" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D112" s="14">
-        <v>41301</v>
-      </c>
-      <c r="E112" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F112" s="15">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113" s="16">
-        <v>7</v>
-      </c>
-      <c r="B113" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C113" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D113" s="14">
-        <v>41302</v>
-      </c>
-      <c r="E113" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F113" s="13"/>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114" s="16">
-        <v>8</v>
-      </c>
-      <c r="B114" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C114" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D114" s="14">
-        <v>41303</v>
-      </c>
-      <c r="E114" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F114" s="13"/>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="A115" s="16">
-        <v>9</v>
-      </c>
-      <c r="B115" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C115" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D115" s="14">
-        <v>41304</v>
-      </c>
-      <c r="E115" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F115" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116" s="16">
-        <v>10</v>
-      </c>
-      <c r="B116" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C116" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116" s="14">
-        <v>41305</v>
-      </c>
-      <c r="E116" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F116" s="15">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" s="16">
-        <v>11</v>
-      </c>
-      <c r="B117" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C117" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D117" s="14">
-        <v>41306</v>
-      </c>
-      <c r="E117" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F117" s="15">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118" s="16">
-        <v>12</v>
-      </c>
-      <c r="B118" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C118" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D118" s="14">
-        <v>41306</v>
-      </c>
-      <c r="E118" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F118" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119" s="16">
-        <v>13</v>
-      </c>
-      <c r="B119" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C119" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D119" s="14">
-        <v>41307</v>
-      </c>
-      <c r="E119" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F119" s="15">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" s="16">
-        <v>14</v>
-      </c>
-      <c r="B120" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="C120" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D120" s="14">
-        <v>41308</v>
-      </c>
-      <c r="E120" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F120" s="13"/>
-    </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="4:4">
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="4:4">
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="4:4">
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="4:4">
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="4:4">
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="4:4">
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="4:4">
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="4:4">
       <c r="D128" s="10"/>
     </row>
     <row r="129" spans="4:4">
@@ -1445,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2918,8 +2876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
@@ -3269,7 +3227,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3309,7 +3267,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="180">
+    <row r="3" spans="1:6" ht="60">
       <c r="A3" s="42" t="s">
         <v>73</v>
       </c>
@@ -3569,7 +3527,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="225">
+    <row r="16" spans="1:6" ht="75">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3889,7 +3847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="345">
+    <row r="32" spans="1:6" ht="90">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -3918,7 +3876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated by Sruti Davis Time: 23:05 Date: 03-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="3645" activeTab="7"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="13200" windowHeight="4548" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,13 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1:P13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -250,6 +251,9 @@
   </si>
   <si>
     <t>MT2012122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing </t>
   </si>
 </sst>
 </file>
@@ -660,12 +664,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4">
@@ -697,14 +701,14 @@
       <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1407,14 +1411,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1447,7 +1451,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="28.8">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1707,7 +1711,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6" ht="28.8">
       <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
@@ -1987,7 +1991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="45">
+    <row r="30" spans="1:6" ht="28.8">
       <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
@@ -2027,7 +2031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="28.8">
       <c r="A32" s="20" t="s">
         <v>15</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30">
+    <row r="34" spans="1:6" ht="28.8">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2100,7 +2104,7 @@
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="29" t="s">
@@ -2490,7 +2494,7 @@
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="33" t="s">
@@ -2880,11 +2884,11 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="4" width="11.7109375" style="34"/>
-    <col min="5" max="5" width="23.85546875" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="11.7109375" style="34"/>
+    <col min="1" max="4" width="11.6640625" style="34"/>
+    <col min="5" max="5" width="23.88671875" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="11.6640625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2952,7 +2956,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7">
       <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
@@ -2986,7 +2990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="28.8">
       <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
@@ -3006,7 +3010,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75">
+    <row r="10" spans="1:7" ht="72">
       <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
@@ -3026,7 +3030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
+    <row r="11" spans="1:7" ht="28.8">
       <c r="A11" s="34" t="s">
         <v>60</v>
       </c>
@@ -3046,7 +3050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="28.8">
       <c r="A12" s="34" t="s">
         <v>60</v>
       </c>
@@ -3063,7 +3067,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30">
+    <row r="13" spans="1:7" ht="28.8">
       <c r="A13" s="34" t="s">
         <v>60</v>
       </c>
@@ -3097,7 +3101,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:7" ht="28.8">
       <c r="A15" s="34" t="s">
         <v>60</v>
       </c>
@@ -3137,7 +3141,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="28.8">
       <c r="A17" s="34" t="s">
         <v>60</v>
       </c>
@@ -3177,7 +3181,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="28.8">
       <c r="A19" s="34" t="s">
         <v>60</v>
       </c>
@@ -3197,7 +3201,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30">
+    <row r="20" spans="1:6" ht="28.8">
       <c r="A20" s="37" t="s">
         <v>60</v>
       </c>
@@ -3230,11 +3234,11 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3267,7 +3271,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60">
+    <row r="3" spans="1:6" ht="57.6">
       <c r="A3" s="42" t="s">
         <v>73</v>
       </c>
@@ -3527,7 +3531,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="75">
+    <row r="16" spans="1:6" ht="43.2">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3847,7 +3851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="90">
+    <row r="32" spans="1:6" ht="86.4">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -3877,10 +3881,16 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F49"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="37" t="s">
@@ -4160,12 +4170,18 @@
       <c r="A15" s="37">
         <v>14</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="B15" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="D15" s="35">
         <v>41308</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="F15" s="36"/>
     </row>
     <row r="16" spans="1:6">

</xml_diff>

<commit_message>
Updated by Sruti Davis Date & Time: 03-02-2013 & 23:22
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:P13"/>
+  <oleSize ref="A9:J21"/>
 </workbook>
 </file>
 
@@ -253,7 +253,7 @@
     <t>MT2012122</t>
   </si>
   <si>
-    <t xml:space="preserve">Nothing </t>
+    <t>Nothing has been done today</t>
   </si>
 </sst>
 </file>
@@ -3880,7 +3880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated by Sruti Davis Dated 4-Feb-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13200" windowHeight="4545" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="13200" windowHeight="2388" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,13 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A11:G16"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -253,6 +254,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nothing </t>
+  </si>
+  <si>
+    <t>Nothing has been done today</t>
   </si>
 </sst>
 </file>
@@ -663,12 +667,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4">
@@ -700,14 +704,14 @@
       <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1410,14 +1414,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1450,7 +1454,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="28.8">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1710,7 +1714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6" ht="28.8">
       <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="45">
+    <row r="30" spans="1:6" ht="28.8">
       <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
@@ -2030,7 +2034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="28.8">
       <c r="A32" s="20" t="s">
         <v>15</v>
       </c>
@@ -2070,7 +2074,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30">
+    <row r="34" spans="1:6" ht="28.8">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2103,7 +2107,7 @@
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="29" t="s">
@@ -2493,7 +2497,7 @@
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="33" t="s">
@@ -2883,11 +2887,11 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="4" width="11.7109375" style="34"/>
-    <col min="5" max="5" width="23.85546875" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="11.7109375" style="34"/>
+    <col min="1" max="4" width="11.6640625" style="34"/>
+    <col min="5" max="5" width="23.88671875" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="11.6640625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2955,7 +2959,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7">
       <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
@@ -2989,7 +2993,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="28.8">
       <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
@@ -3009,7 +3013,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75">
+    <row r="10" spans="1:7" ht="72">
       <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
@@ -3029,7 +3033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
+    <row r="11" spans="1:7" ht="28.8">
       <c r="A11" s="34" t="s">
         <v>60</v>
       </c>
@@ -3049,7 +3053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="28.8">
       <c r="A12" s="34" t="s">
         <v>60</v>
       </c>
@@ -3066,7 +3070,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30">
+    <row r="13" spans="1:7" ht="28.8">
       <c r="A13" s="34" t="s">
         <v>60</v>
       </c>
@@ -3100,7 +3104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:7" ht="28.8">
       <c r="A15" s="34" t="s">
         <v>60</v>
       </c>
@@ -3140,7 +3144,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="28.8">
       <c r="A17" s="34" t="s">
         <v>60</v>
       </c>
@@ -3180,7 +3184,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="28.8">
       <c r="A19" s="34" t="s">
         <v>60</v>
       </c>
@@ -3200,7 +3204,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30">
+    <row r="20" spans="1:6" ht="28.8">
       <c r="A20" s="37" t="s">
         <v>60</v>
       </c>
@@ -3229,15 +3233,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3270,7 +3274,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60">
+    <row r="3" spans="1:6" ht="57.6">
       <c r="A3" s="42" t="s">
         <v>73</v>
       </c>
@@ -3530,7 +3534,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="75">
+    <row r="16" spans="1:6" ht="43.2">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3850,7 +3854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="90">
+    <row r="32" spans="1:6" ht="86.4">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -3899,16 +3903,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="2" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4207,12 +4211,18 @@
       <c r="A16" s="37">
         <v>15</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="B16" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="D16" s="35">
         <v>41309</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="42" t="s">
+        <v>76</v>
+      </c>
       <c r="F16" s="36"/>
     </row>
     <row r="17" spans="1:6">

</xml_diff>

<commit_message>
updated by sravani 4/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="13200" windowHeight="2388" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2475" windowWidth="13200" windowHeight="2385" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,12 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A11:G16"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -257,6 +256,12 @@
   </si>
   <si>
     <t>Nothing has been done today</t>
+  </si>
+  <si>
+    <t>Mini Project</t>
+  </si>
+  <si>
+    <t>Coding part for the admin section of student profile.</t>
   </si>
 </sst>
 </file>
@@ -667,12 +672,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
-    <col min="4" max="4" width="42.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4">
@@ -704,14 +709,14 @@
       <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1414,14 +1419,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1454,7 +1459,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1714,7 +1719,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
@@ -1994,7 +1999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8">
+    <row r="30" spans="1:6" ht="45">
       <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
@@ -2034,7 +2039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="28.8">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="20" t="s">
         <v>15</v>
       </c>
@@ -2074,7 +2079,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2107,7 +2112,7 @@
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="29" t="s">
@@ -2497,7 +2502,7 @@
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="33" t="s">
@@ -2887,11 +2892,11 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="11.6640625" style="34"/>
-    <col min="5" max="5" width="23.88671875" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="11.6640625" style="34"/>
+    <col min="1" max="4" width="11.7109375" style="34"/>
+    <col min="5" max="5" width="23.85546875" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="11.7109375" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2959,7 +2964,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
@@ -2993,7 +2998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
@@ -3013,7 +3018,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="72">
+    <row r="10" spans="1:7" ht="75">
       <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
@@ -3033,7 +3038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8">
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="34" t="s">
         <v>60</v>
       </c>
@@ -3053,7 +3058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="34" t="s">
         <v>60</v>
       </c>
@@ -3070,7 +3075,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="34" t="s">
         <v>60</v>
       </c>
@@ -3104,7 +3109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8">
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="34" t="s">
         <v>60</v>
       </c>
@@ -3144,7 +3149,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="34" t="s">
         <v>60</v>
       </c>
@@ -3184,7 +3189,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="34" t="s">
         <v>60</v>
       </c>
@@ -3204,7 +3209,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="37" t="s">
         <v>60</v>
       </c>
@@ -3231,17 +3236,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3274,7 +3279,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.6">
+    <row r="3" spans="1:6" ht="60">
       <c r="A3" s="42" t="s">
         <v>73</v>
       </c>
@@ -3534,7 +3539,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2">
+    <row r="16" spans="1:6" ht="75">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3854,7 +3859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="86.4">
+    <row r="32" spans="1:6" ht="90">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -3874,7 +3879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="42" t="s">
         <v>73</v>
       </c>
@@ -3885,13 +3890,33 @@
         <v>40942</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="F33" s="44">
-        <v>0</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30">
+      <c r="A34" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="43">
+        <v>40943</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="44">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3903,16 +3928,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="49.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="2" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
updated by alpna date 4/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2475" windowWidth="13200" windowHeight="2385" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2475" windowWidth="13200" windowHeight="2385" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1012,7 +1012,22 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="D16" s="1"/>
+      <c r="A16" s="37">
+        <v>15</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="43">
+        <v>41309</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="4:4">
       <c r="D17" s="1"/>
@@ -3238,7 +3253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Done BY: B S Deepthi Date: 06-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6210" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6210" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -274,13 +274,19 @@
   </si>
   <si>
     <t>Coding for Student Profile Project</t>
+  </si>
+  <si>
+    <t>Changed some database tables Friend, User_interest for the design of My Friends page</t>
+  </si>
+  <si>
+    <t>Done with My Friend's Screen along with the pagination functionality.Committed the changes to SVN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,7 +479,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -508,7 +513,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -684,14 +688,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C5:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -699,7 +703,7 @@
     <col min="4" max="4" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4">
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -707,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -721,14 +725,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView topLeftCell="C10" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
@@ -738,7 +742,7 @@
     <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
@@ -758,7 +762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -778,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -796,7 +800,7 @@
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -816,7 +820,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -836,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -856,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -876,7 +880,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -894,7 +898,7 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -912,7 +916,7 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="16">
         <v>9</v>
       </c>
@@ -932,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -952,7 +956,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -972,7 +976,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="16">
         <v>12</v>
       </c>
@@ -992,7 +996,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="16">
         <v>13</v>
       </c>
@@ -1012,7 +1016,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="16">
         <v>14</v>
       </c>
@@ -1030,7 +1034,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="37">
         <v>15</v>
       </c>
@@ -1048,7 +1052,7 @@
       </c>
       <c r="F16" s="42"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>16</v>
       </c>
@@ -1068,88 +1072,88 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="D18" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="D49" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="4"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1157,116 +1161,116 @@
       <c r="E53" s="7"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="C54" s="1"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="C56" s="1"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="C59" s="1"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="C60" s="1"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="C61" s="1"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="C63" s="1"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="C64" s="1"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:6">
       <c r="C65" s="1"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:6">
       <c r="C66" s="1"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:6">
       <c r="C67" s="1"/>
       <c r="E67" s="5"/>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6">
       <c r="C68" s="1"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:6">
       <c r="C69" s="1"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:6">
       <c r="C70" s="1"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:6">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:6">
       <c r="C72" s="1"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:6">
       <c r="C73" s="1"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:6">
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:6">
       <c r="C75" s="1"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:6">
       <c r="C76" s="1"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:6">
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:6">
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:6">
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:6">
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="C81" s="1"/>
       <c r="E81" s="5"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="C83" s="1"/>
       <c r="E83" s="5"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="12"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -1274,7 +1278,7 @@
       <c r="E87" s="9"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="12"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -1282,7 +1286,7 @@
       <c r="E88" s="9"/>
       <c r="F88" s="11"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="12"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -1290,7 +1294,7 @@
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="12"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -1298,7 +1302,7 @@
       <c r="E90" s="9"/>
       <c r="F90" s="11"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="12"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -1306,7 +1310,7 @@
       <c r="E91" s="9"/>
       <c r="F91" s="11"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="12"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -1314,7 +1318,7 @@
       <c r="E92" s="9"/>
       <c r="F92" s="11"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="12"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -1322,7 +1326,7 @@
       <c r="E93" s="9"/>
       <c r="F93" s="11"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="12"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -1330,7 +1334,7 @@
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="12"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -1338,7 +1342,7 @@
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="12"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -1346,7 +1350,7 @@
       <c r="E96" s="9"/>
       <c r="F96" s="11"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="12"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -1354,7 +1358,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="11"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="12"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -1362,7 +1366,7 @@
       <c r="E98" s="9"/>
       <c r="F98" s="11"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="12"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -1370,7 +1374,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="11"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="12"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -1378,7 +1382,7 @@
       <c r="E100" s="9"/>
       <c r="F100" s="11"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="12"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -1386,7 +1390,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -1394,66 +1398,66 @@
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103"/>
       <c r="C103" s="1"/>
       <c r="D103" s="10"/>
       <c r="F103" s="6"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104"/>
       <c r="C104" s="1"/>
       <c r="D104" s="10"/>
       <c r="F104" s="6"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105"/>
       <c r="C105" s="1"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:4">
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:4">
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:4">
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:4">
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:4">
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:4">
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:4">
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:4">
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:4">
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:4">
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:4">
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:4">
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:4">
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:4">
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:4">
       <c r="D135" s="10"/>
     </row>
   </sheetData>
@@ -1463,14 +1467,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -1480,7 +1484,7 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -1490,7 +1494,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -1510,7 +1514,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1530,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="20" t="s">
         <v>15</v>
       </c>
@@ -1570,7 +1574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="20" t="s">
         <v>15</v>
       </c>
@@ -1590,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="20" t="s">
         <v>15</v>
       </c>
@@ -1610,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
         <v>15</v>
       </c>
@@ -1630,7 +1634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="20" t="s">
         <v>15</v>
       </c>
@@ -1650,7 +1654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="20" t="s">
         <v>15</v>
       </c>
@@ -1670,7 +1674,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="20" t="s">
         <v>15</v>
       </c>
@@ -1690,7 +1694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
@@ -1710,7 +1714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
         <v>15</v>
       </c>
@@ -1730,7 +1734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="20" t="s">
         <v>15</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="20" t="s">
         <v>15</v>
       </c>
@@ -1770,7 +1774,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
@@ -1790,7 +1794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="20" t="s">
         <v>15</v>
       </c>
@@ -1810,7 +1814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="20" t="s">
         <v>15</v>
       </c>
@@ -1830,7 +1834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="20" t="s">
         <v>15</v>
       </c>
@@ -1850,7 +1854,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="20" t="s">
         <v>15</v>
       </c>
@@ -1870,7 +1874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="20" t="s">
         <v>15</v>
       </c>
@@ -1890,7 +1894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="20" t="s">
         <v>15</v>
       </c>
@@ -1930,7 +1934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="20" t="s">
         <v>15</v>
       </c>
@@ -1950,7 +1954,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="20" t="s">
         <v>15</v>
       </c>
@@ -1970,7 +1974,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="20" t="s">
         <v>15</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="20" t="s">
         <v>15</v>
       </c>
@@ -2010,7 +2014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="20" t="s">
         <v>15</v>
       </c>
@@ -2030,7 +2034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="20" t="s">
         <v>15</v>
       </c>
@@ -2050,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="45">
       <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
@@ -2070,7 +2074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="20" t="s">
         <v>15</v>
       </c>
@@ -2090,7 +2094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="20" t="s">
         <v>15</v>
       </c>
@@ -2110,7 +2114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
@@ -2130,7 +2134,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2148,6 +2152,46 @@
       </c>
       <c r="F34" s="36">
         <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="43">
+        <v>41309</v>
+      </c>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="43">
+        <v>41310</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2156,14 +2200,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
@@ -2183,7 +2227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="29">
         <v>1</v>
       </c>
@@ -2203,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -2221,7 +2265,7 @@
       </c>
       <c r="F3" s="26"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -2241,7 +2285,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="29">
         <v>4</v>
       </c>
@@ -2261,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="29">
         <v>5</v>
       </c>
@@ -2281,7 +2325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="29">
         <v>6</v>
       </c>
@@ -2301,7 +2345,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="29">
         <v>7</v>
       </c>
@@ -2319,7 +2363,7 @@
       </c>
       <c r="F8" s="26"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="29">
         <v>8</v>
       </c>
@@ -2337,7 +2381,7 @@
       </c>
       <c r="F9" s="26"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="29">
         <v>9</v>
       </c>
@@ -2357,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="29">
         <v>10</v>
       </c>
@@ -2377,7 +2421,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="29">
         <v>11</v>
       </c>
@@ -2397,7 +2441,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="29">
         <v>12</v>
       </c>
@@ -2417,7 +2461,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="29">
         <v>13</v>
       </c>
@@ -2437,7 +2481,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="29">
         <v>14</v>
       </c>
@@ -2449,7 +2493,7 @@
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -2457,85 +2501,85 @@
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" s="27"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" s="27"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" s="27"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" s="27"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" s="27"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" s="27"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" s="27"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4">
       <c r="D32" s="27"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="27"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="27"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="27"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="27"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="27"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="27"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="27"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="27"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="27"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="27"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="27"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="27"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="27"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="27"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="27"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="27"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="27"/>
     </row>
   </sheetData>
@@ -2544,16 +2588,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="33" t="s">
         <v>7</v>
       </c>
@@ -2573,7 +2617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="33">
         <v>1</v>
       </c>
@@ -2593,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="33">
         <v>2</v>
       </c>
@@ -2611,7 +2655,7 @@
       </c>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="33">
         <v>3</v>
       </c>
@@ -2631,7 +2675,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -2651,7 +2695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="33">
         <v>5</v>
       </c>
@@ -2671,7 +2715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="33">
         <v>6</v>
       </c>
@@ -2691,7 +2735,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="33">
         <v>7</v>
       </c>
@@ -2709,7 +2753,7 @@
       </c>
       <c r="F8" s="30"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="33">
         <v>8</v>
       </c>
@@ -2727,7 +2771,7 @@
       </c>
       <c r="F9" s="30"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="33">
         <v>9</v>
       </c>
@@ -2747,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="33">
         <v>10</v>
       </c>
@@ -2767,7 +2811,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="33">
         <v>11</v>
       </c>
@@ -2787,7 +2831,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="33">
         <v>12</v>
       </c>
@@ -2807,7 +2851,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -2827,7 +2871,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="33">
         <v>14</v>
       </c>
@@ -2839,7 +2883,7 @@
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -2847,85 +2891,85 @@
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" s="31"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" s="31"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" s="31"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" s="31"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4">
       <c r="D32" s="31"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="31"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="31"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="31"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="31"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="31"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="31"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="31"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="31"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="31"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="31"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="31"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="31"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="31"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="31"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="31"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="31"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="31"/>
     </row>
   </sheetData>
@@ -2934,14 +2978,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="11.7109375" style="34"/>
     <col min="4" max="4" width="27.5703125" style="34" customWidth="1"/>
@@ -2949,7 +2993,7 @@
     <col min="6" max="16384" width="11.7109375" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2969,7 +3013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="21"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2977,7 +3021,7 @@
       <c r="E2" s="40"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="21"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -2985,7 +3029,7 @@
       <c r="E3" s="40"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="21"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -2993,7 +3037,7 @@
       <c r="E4" s="40"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="21"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -3001,7 +3045,7 @@
       <c r="E5" s="40"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="34" t="s">
         <v>60</v>
       </c>
@@ -3014,7 +3058,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
@@ -3034,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="34" t="s">
         <v>60</v>
       </c>
@@ -3048,7 +3092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
@@ -3068,7 +3112,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="75">
       <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
@@ -3088,7 +3132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="34" t="s">
         <v>60</v>
       </c>
@@ -3108,7 +3152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="34" t="s">
         <v>60</v>
       </c>
@@ -3125,7 +3169,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="34" t="s">
         <v>60</v>
       </c>
@@ -3145,7 +3189,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="34" t="s">
         <v>60</v>
       </c>
@@ -3159,7 +3203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="34" t="s">
         <v>60</v>
       </c>
@@ -3179,7 +3223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="34" t="s">
         <v>60</v>
       </c>
@@ -3199,7 +3243,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="34" t="s">
         <v>60</v>
       </c>
@@ -3219,7 +3263,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="34" t="s">
         <v>60</v>
       </c>
@@ -3239,7 +3283,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="34" t="s">
         <v>60</v>
       </c>
@@ -3259,7 +3303,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="37" t="s">
         <v>60</v>
       </c>
@@ -3279,7 +3323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30">
       <c r="A21" s="37" t="s">
         <v>60</v>
       </c>
@@ -3299,7 +3343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="37" t="s">
         <v>60</v>
       </c>
@@ -3325,21 +3369,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" customWidth="1"/>
     <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="45" t="s">
         <v>72</v>
       </c>
@@ -3349,7 +3393,7 @@
       <c r="E1" s="42"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
@@ -3369,7 +3413,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="60">
       <c r="A3" s="42" t="s">
         <v>73</v>
       </c>
@@ -3389,7 +3433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="42" t="s">
         <v>73</v>
       </c>
@@ -3409,7 +3453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="42" t="s">
         <v>73</v>
       </c>
@@ -3429,7 +3473,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="42" t="s">
         <v>73</v>
       </c>
@@ -3449,7 +3493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="42" t="s">
         <v>73</v>
       </c>
@@ -3469,7 +3513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="42" t="s">
         <v>73</v>
       </c>
@@ -3489,7 +3533,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="42" t="s">
         <v>73</v>
       </c>
@@ -3509,7 +3553,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="42" t="s">
         <v>73</v>
       </c>
@@ -3529,7 +3573,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="42" t="s">
         <v>73</v>
       </c>
@@ -3549,7 +3593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="42" t="s">
         <v>73</v>
       </c>
@@ -3569,7 +3613,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="42" t="s">
         <v>73</v>
       </c>
@@ -3589,7 +3633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="42" t="s">
         <v>73</v>
       </c>
@@ -3609,7 +3653,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="42" t="s">
         <v>73</v>
       </c>
@@ -3629,7 +3673,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="75">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3649,7 +3693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="42" t="s">
         <v>73</v>
       </c>
@@ -3669,7 +3713,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="42" t="s">
         <v>73</v>
       </c>
@@ -3689,7 +3733,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="42" t="s">
         <v>73</v>
       </c>
@@ -3709,7 +3753,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="42" t="s">
         <v>73</v>
       </c>
@@ -3729,7 +3773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="42" t="s">
         <v>73</v>
       </c>
@@ -3749,7 +3793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="42" t="s">
         <v>73</v>
       </c>
@@ -3769,7 +3813,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="42" t="s">
         <v>73</v>
       </c>
@@ -3789,7 +3833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="42" t="s">
         <v>73</v>
       </c>
@@ -3809,7 +3853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="42" t="s">
         <v>73</v>
       </c>
@@ -3829,7 +3873,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="42" t="s">
         <v>73</v>
       </c>
@@ -3849,7 +3893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="42" t="s">
         <v>73</v>
       </c>
@@ -3869,7 +3913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="42" t="s">
         <v>73</v>
       </c>
@@ -3889,7 +3933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="42" t="s">
         <v>73</v>
       </c>
@@ -3909,7 +3953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="42" t="s">
         <v>73</v>
       </c>
@@ -3929,7 +3973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="42" t="s">
         <v>73</v>
       </c>
@@ -3949,7 +3993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="90">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -3969,7 +4013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="42" t="s">
         <v>73</v>
       </c>
@@ -3989,7 +4033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="42" t="s">
         <v>73</v>
       </c>
@@ -4009,7 +4053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="42" t="s">
         <v>73</v>
       </c>
@@ -4035,14 +4079,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -4050,7 +4094,7 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
@@ -4070,7 +4114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -4090,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -4108,7 +4152,7 @@
       </c>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -4128,7 +4172,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -4148,7 +4192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -4168,7 +4212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -4188,7 +4232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="37">
         <v>7</v>
       </c>
@@ -4206,7 +4250,7 @@
       </c>
       <c r="F8" s="36"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="37">
         <v>8</v>
       </c>
@@ -4224,7 +4268,7 @@
       </c>
       <c r="F9" s="36"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="37">
         <v>9</v>
       </c>
@@ -4244,7 +4288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="37">
         <v>10</v>
       </c>
@@ -4264,7 +4308,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="37">
         <v>11</v>
       </c>
@@ -4284,7 +4328,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="37">
         <v>12</v>
       </c>
@@ -4304,7 +4348,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="37">
         <v>13</v>
       </c>
@@ -4324,7 +4368,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="37">
         <v>14</v>
       </c>
@@ -4342,7 +4386,7 @@
       </c>
       <c r="F15" s="36"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="37">
         <v>15</v>
       </c>
@@ -4360,7 +4404,7 @@
       </c>
       <c r="F16" s="36"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>16</v>
       </c>
@@ -4372,7 +4416,7 @@
       <c r="E17" s="34"/>
       <c r="F17" s="36"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>17</v>
       </c>
@@ -4384,7 +4428,7 @@
       <c r="E18" s="34"/>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="37">
         <v>18</v>
       </c>
@@ -4396,7 +4440,7 @@
       <c r="E19" s="34"/>
       <c r="F19" s="36"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="37">
         <v>19</v>
       </c>
@@ -4406,7 +4450,7 @@
       <c r="E20" s="34"/>
       <c r="F20" s="34"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="37">
         <v>20</v>
       </c>
@@ -4416,7 +4460,7 @@
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="37">
         <v>21</v>
       </c>
@@ -4426,7 +4470,7 @@
       <c r="E22" s="34"/>
       <c r="F22" s="34"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="37">
         <v>22</v>
       </c>
@@ -4436,7 +4480,7 @@
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="37">
         <v>23</v>
       </c>
@@ -4446,7 +4490,7 @@
       <c r="E24" s="34"/>
       <c r="F24" s="34"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="37">
         <v>24</v>
       </c>
@@ -4456,7 +4500,7 @@
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="37">
         <v>25</v>
       </c>
@@ -4466,7 +4510,7 @@
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="37">
         <v>26</v>
       </c>
@@ -4476,7 +4520,7 @@
       <c r="E27" s="34"/>
       <c r="F27" s="34"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="37">
         <v>27</v>
       </c>
@@ -4486,7 +4530,7 @@
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="37">
         <v>28</v>
       </c>
@@ -4496,7 +4540,7 @@
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="37">
         <v>29</v>
       </c>
@@ -4506,7 +4550,7 @@
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="37">
         <v>30</v>
       </c>
@@ -4516,7 +4560,7 @@
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="37">
         <v>31</v>
       </c>
@@ -4526,87 +4570,87 @@
       <c r="E32" s="34"/>
       <c r="F32" s="34"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="37">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="37">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="37">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="37">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="37">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="37">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="37">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="37">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="37">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="37">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="37">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="37">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="37">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="37">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="37">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="37">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
updated by sravani date: 6/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6210" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6210" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -280,6 +280,42 @@
   </si>
   <si>
     <t>Done with My Friend's Screen along with the pagination functionality.Committed the changes to SVN</t>
+  </si>
+  <si>
+    <t>know your friend "ebay"</t>
+  </si>
+  <si>
+    <t>updated know your friend "ebay"</t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>Preparing the document 
+"Know your friend" along with 
+Team mates</t>
+  </si>
+  <si>
+    <t>Requirements for Ebay(Team meeting)</t>
+  </si>
+  <si>
+    <t>created account in ebay for better understanding of ebay functionalities</t>
+  </si>
+  <si>
+    <t>Discussed the functionalities of ebay that are to be implemented.</t>
+  </si>
+  <si>
+    <t>Division of implementation of functionalities among team mates and Clarification of doubts in mini project</t>
+  </si>
+  <si>
+    <t>Review of usecases, interaction 
+stories, test transactions by sir</t>
+  </si>
+  <si>
+    <t>Finalized the Database schema 
+by discussing with 
+Teammembers and 
+mentor</t>
   </si>
 </sst>
 </file>
@@ -323,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -390,6 +426,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1470,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -3370,14 +3409,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" customWidth="1"/>
     <col min="5" max="5" width="30.140625" customWidth="1"/>
@@ -3413,7 +3452,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60">
+    <row r="3" spans="1:6">
       <c r="A3" s="42" t="s">
         <v>73</v>
       </c>
@@ -3427,7 +3466,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="F3" s="44">
         <v>1</v>
@@ -3444,13 +3483,13 @@
         <v>40913</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F4" s="44">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3473,7 +3512,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="42" t="s">
         <v>73</v>
       </c>
@@ -3486,14 +3525,14 @@
       <c r="D6" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="42" t="s">
-        <v>31</v>
+      <c r="E6" s="46" t="s">
+        <v>86</v>
       </c>
       <c r="F6" s="44">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="45">
       <c r="A7" s="42" t="s">
         <v>73</v>
       </c>
@@ -3504,10 +3543,10 @@
         <v>40916</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>33</v>
+        <v>89</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>88</v>
       </c>
       <c r="F7" s="44">
         <v>2</v>
@@ -3633,7 +3672,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="42" t="s">
         <v>73</v>
       </c>
@@ -3644,10 +3683,10 @@
         <v>40923</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>18</v>
+        <v>87</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>90</v>
       </c>
       <c r="F14" s="47" t="s">
         <v>32</v>
@@ -3673,7 +3712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="75">
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3684,10 +3723,10 @@
         <v>40925</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="F16" s="44">
         <v>3</v>
@@ -3784,13 +3823,13 @@
         <v>40930</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="F21" s="47">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3824,7 +3863,7 @@
         <v>40932</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E23" s="42" t="s">
         <v>37</v>
@@ -3944,16 +3983,16 @@
         <v>40938</v>
       </c>
       <c r="D29" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="42" t="s">
         <v>42</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>43</v>
       </c>
       <c r="F29" s="44">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" ht="30">
       <c r="A30" s="42" t="s">
         <v>73</v>
       </c>
@@ -3966,14 +4005,14 @@
       <c r="D30" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="44">
-        <v>1.5</v>
+      <c r="E30" s="50" t="s">
+        <v>93</v>
       </c>
       <c r="F30" s="44">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="60">
       <c r="A31" s="42" t="s">
         <v>73</v>
       </c>
@@ -3984,16 +4023,16 @@
         <v>40940</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="42" t="s">
-        <v>46</v>
+        <v>27</v>
+      </c>
+      <c r="E31" s="46" t="s">
+        <v>94</v>
       </c>
       <c r="F31" s="44">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="90">
+    <row r="32" spans="1:6" ht="60">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -4004,13 +4043,13 @@
         <v>40941</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="F32" s="44">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30">
@@ -4070,6 +4109,26 @@
         <v>18</v>
       </c>
       <c r="F35" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="43">
+        <v>40945</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="44">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated by Sruti Davis
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6210" firstSheet="1" activeTab="6"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="13200" windowHeight="2076" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,13 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A11:G16"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -734,12 +735,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4">
@@ -771,14 +772,14 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1513,14 +1514,14 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1553,7 +1554,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="28.8">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6" ht="28.8">
       <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="45">
+    <row r="30" spans="1:6" ht="28.8">
       <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
@@ -2133,7 +2134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="28.8">
       <c r="A32" s="20" t="s">
         <v>15</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30">
+    <row r="34" spans="1:6" ht="28.8">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2244,7 +2245,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="29" t="s">
@@ -2634,7 +2635,7 @@
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="33" t="s">
@@ -3024,12 +3025,12 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="11.7109375" style="34"/>
-    <col min="4" max="4" width="27.5703125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="11.7109375" style="34"/>
+    <col min="1" max="3" width="11.6640625" style="34"/>
+    <col min="4" max="4" width="27.5546875" style="34" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="11.6640625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3097,7 +3098,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7">
       <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="28.8">
       <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
@@ -3151,7 +3152,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75">
+    <row r="10" spans="1:7" ht="72">
       <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
+    <row r="11" spans="1:7" ht="28.8">
       <c r="A11" s="34" t="s">
         <v>60</v>
       </c>
@@ -3191,7 +3192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="28.8">
       <c r="A12" s="34" t="s">
         <v>60</v>
       </c>
@@ -3208,7 +3209,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30">
+    <row r="13" spans="1:7" ht="28.8">
       <c r="A13" s="34" t="s">
         <v>60</v>
       </c>
@@ -3242,7 +3243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:7" ht="28.8">
       <c r="A15" s="34" t="s">
         <v>60</v>
       </c>
@@ -3282,7 +3283,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="28.8">
       <c r="A17" s="34" t="s">
         <v>60</v>
       </c>
@@ -3322,7 +3323,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="28.8">
       <c r="A19" s="34" t="s">
         <v>60</v>
       </c>
@@ -3342,7 +3343,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30">
+    <row r="20" spans="1:6" ht="28.8">
       <c r="A20" s="37" t="s">
         <v>60</v>
       </c>
@@ -3362,7 +3363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30">
+    <row r="21" spans="1:6">
       <c r="A21" s="37" t="s">
         <v>60</v>
       </c>
@@ -3382,7 +3383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6">
       <c r="A22" s="37" t="s">
         <v>60</v>
       </c>
@@ -3411,15 +3412,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3512,7 +3513,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30">
+    <row r="6" spans="1:6">
       <c r="A6" s="42" t="s">
         <v>73</v>
       </c>
@@ -3532,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45">
+    <row r="7" spans="1:6" ht="43.2">
       <c r="A7" s="42" t="s">
         <v>73</v>
       </c>
@@ -3672,7 +3673,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:6" ht="43.2">
       <c r="A14" s="42" t="s">
         <v>73</v>
       </c>
@@ -3712,7 +3713,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45">
+    <row r="16" spans="1:6" ht="28.8">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3992,7 +3993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30">
+    <row r="30" spans="1:6" ht="28.8">
       <c r="A30" s="42" t="s">
         <v>73</v>
       </c>
@@ -4012,7 +4013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60">
+    <row r="31" spans="1:6" ht="57.6">
       <c r="A31" s="42" t="s">
         <v>73</v>
       </c>
@@ -4032,7 +4033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="60">
+    <row r="32" spans="1:6" ht="57.6">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30">
+    <row r="33" spans="1:6" ht="28.8">
       <c r="A33" s="42" t="s">
         <v>73</v>
       </c>
@@ -4072,7 +4073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30">
+    <row r="34" spans="1:6" ht="28.8">
       <c r="A34" s="42" t="s">
         <v>73</v>
       </c>
@@ -4141,16 +4142,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="2" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4467,24 +4468,36 @@
       <c r="A17" s="37">
         <v>16</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
+      <c r="B17" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="D17" s="35">
         <v>41310</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="F17" s="36"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>17</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="B18" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="D18" s="35">
         <v>41311</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="E18" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="F18" s="36"/>
     </row>
     <row r="19" spans="1:6">

</xml_diff>

<commit_message>
updated by Priyasmita 6-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13200" windowHeight="2070" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16485" windowHeight="6390" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,11 +17,12 @@
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A7:O25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -317,12 +318,42 @@
 Teammembers and 
 mentor</t>
   </si>
+  <si>
+    <t>MT2012106</t>
+  </si>
+  <si>
+    <t>MT2012107</t>
+  </si>
+  <si>
+    <t>MT2012108</t>
+  </si>
+  <si>
+    <t>MT2012109</t>
+  </si>
+  <si>
+    <t>MT2012110</t>
+  </si>
+  <si>
+    <t>MT2012111</t>
+  </si>
+  <si>
+    <t>MT2012112</t>
+  </si>
+  <si>
+    <t>MT2012113</t>
+  </si>
+  <si>
+    <t>MT2012114</t>
+  </si>
+  <si>
+    <t>coding for student profile</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,7 +549,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -553,7 +583,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -729,14 +758,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C5:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -744,7 +773,7 @@
     <col min="4" max="4" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4">
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -752,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -766,14 +795,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
@@ -783,7 +812,7 @@
     <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
@@ -803,7 +832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -823,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -841,7 +870,7 @@
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -861,7 +890,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -881,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -901,7 +930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -921,7 +950,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -939,7 +968,7 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -957,7 +986,7 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="16">
         <v>9</v>
       </c>
@@ -977,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -997,7 +1026,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -1017,7 +1046,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="16">
         <v>12</v>
       </c>
@@ -1037,7 +1066,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="16">
         <v>13</v>
       </c>
@@ -1057,7 +1086,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="16">
         <v>14</v>
       </c>
@@ -1075,7 +1104,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="37">
         <v>15</v>
       </c>
@@ -1093,7 +1122,7 @@
       </c>
       <c r="F16" s="42"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>16</v>
       </c>
@@ -1113,7 +1142,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>17</v>
       </c>
@@ -1133,85 +1162,85 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="D49" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="4"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1219,116 +1248,116 @@
       <c r="E53" s="7"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="C54" s="1"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="C56" s="1"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="C59" s="1"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="C60" s="1"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="C61" s="1"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="C63" s="1"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="C64" s="1"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:6">
       <c r="C65" s="1"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:6">
       <c r="C66" s="1"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:6">
       <c r="C67" s="1"/>
       <c r="E67" s="5"/>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6">
       <c r="C68" s="1"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:6">
       <c r="C69" s="1"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:6">
       <c r="C70" s="1"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:6">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:6">
       <c r="C72" s="1"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:6">
       <c r="C73" s="1"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:6">
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:6">
       <c r="C75" s="1"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:6">
       <c r="C76" s="1"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:6">
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:6">
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:6">
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:6">
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="C81" s="1"/>
       <c r="E81" s="5"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="C83" s="1"/>
       <c r="E83" s="5"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="12"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -1336,7 +1365,7 @@
       <c r="E87" s="9"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="12"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -1344,7 +1373,7 @@
       <c r="E88" s="9"/>
       <c r="F88" s="11"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="12"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -1352,7 +1381,7 @@
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="12"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -1360,7 +1389,7 @@
       <c r="E90" s="9"/>
       <c r="F90" s="11"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="12"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -1368,7 +1397,7 @@
       <c r="E91" s="9"/>
       <c r="F91" s="11"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="12"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -1376,7 +1405,7 @@
       <c r="E92" s="9"/>
       <c r="F92" s="11"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="12"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -1384,7 +1413,7 @@
       <c r="E93" s="9"/>
       <c r="F93" s="11"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="12"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -1392,7 +1421,7 @@
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="12"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -1400,7 +1429,7 @@
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="12"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -1408,7 +1437,7 @@
       <c r="E96" s="9"/>
       <c r="F96" s="11"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="12"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -1416,7 +1445,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="11"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="12"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -1424,7 +1453,7 @@
       <c r="E98" s="9"/>
       <c r="F98" s="11"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="12"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -1432,7 +1461,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="11"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="12"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -1440,7 +1469,7 @@
       <c r="E100" s="9"/>
       <c r="F100" s="11"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="12"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -1448,7 +1477,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -1456,66 +1485,66 @@
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103"/>
       <c r="C103" s="1"/>
       <c r="D103" s="10"/>
       <c r="F103" s="6"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104"/>
       <c r="C104" s="1"/>
       <c r="D104" s="10"/>
       <c r="F104" s="6"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105"/>
       <c r="C105" s="1"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:4">
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:4">
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:4">
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:4">
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:4">
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:4">
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:4">
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:4">
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:4">
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:4">
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:4">
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:4">
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:4">
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:4">
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:4">
       <c r="D135" s="10"/>
     </row>
   </sheetData>
@@ -1525,14 +1554,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -1542,7 +1571,7 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -1552,7 +1581,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -1572,7 +1601,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1592,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
@@ -1612,7 +1641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="20" t="s">
         <v>15</v>
       </c>
@@ -1632,7 +1661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="20" t="s">
         <v>15</v>
       </c>
@@ -1652,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="20" t="s">
         <v>15</v>
       </c>
@@ -1672,7 +1701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
         <v>15</v>
       </c>
@@ -1692,7 +1721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="20" t="s">
         <v>15</v>
       </c>
@@ -1712,7 +1741,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="20" t="s">
         <v>15</v>
       </c>
@@ -1732,7 +1761,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="20" t="s">
         <v>15</v>
       </c>
@@ -1752,7 +1781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
@@ -1772,7 +1801,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
         <v>15</v>
       </c>
@@ -1792,7 +1821,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="20" t="s">
         <v>15</v>
       </c>
@@ -1812,7 +1841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="20" t="s">
         <v>15</v>
       </c>
@@ -1832,7 +1861,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
@@ -1852,7 +1881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="20" t="s">
         <v>15</v>
       </c>
@@ -1872,7 +1901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="20" t="s">
         <v>15</v>
       </c>
@@ -1892,7 +1921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="20" t="s">
         <v>15</v>
       </c>
@@ -1912,7 +1941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="20" t="s">
         <v>15</v>
       </c>
@@ -1932,7 +1961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="20" t="s">
         <v>15</v>
       </c>
@@ -1952,7 +1981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
@@ -1972,7 +2001,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="20" t="s">
         <v>15</v>
       </c>
@@ -1992,7 +2021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="20" t="s">
         <v>15</v>
       </c>
@@ -2012,7 +2041,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="20" t="s">
         <v>15</v>
       </c>
@@ -2032,7 +2061,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="20" t="s">
         <v>15</v>
       </c>
@@ -2052,7 +2081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="20" t="s">
         <v>15</v>
       </c>
@@ -2072,7 +2101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="20" t="s">
         <v>15</v>
       </c>
@@ -2092,7 +2121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="20" t="s">
         <v>15</v>
       </c>
@@ -2112,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="45">
       <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
@@ -2132,7 +2161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="20" t="s">
         <v>15</v>
       </c>
@@ -2152,7 +2181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="20" t="s">
         <v>15</v>
       </c>
@@ -2172,7 +2201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
@@ -2192,7 +2221,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2212,7 +2241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -2232,7 +2261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -2258,14 +2287,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
@@ -2285,7 +2314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="29">
         <v>1</v>
       </c>
@@ -2305,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -2323,7 +2352,7 @@
       </c>
       <c r="F3" s="26"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -2343,7 +2372,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="29">
         <v>4</v>
       </c>
@@ -2363,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="29">
         <v>5</v>
       </c>
@@ -2383,7 +2412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="29">
         <v>6</v>
       </c>
@@ -2403,7 +2432,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="29">
         <v>7</v>
       </c>
@@ -2421,7 +2450,7 @@
       </c>
       <c r="F8" s="26"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="29">
         <v>8</v>
       </c>
@@ -2439,7 +2468,7 @@
       </c>
       <c r="F9" s="26"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="29">
         <v>9</v>
       </c>
@@ -2459,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="29">
         <v>10</v>
       </c>
@@ -2479,7 +2508,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="29">
         <v>11</v>
       </c>
@@ -2499,7 +2528,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="29">
         <v>12</v>
       </c>
@@ -2519,7 +2548,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="29">
         <v>13</v>
       </c>
@@ -2539,7 +2568,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="29">
         <v>14</v>
       </c>
@@ -2551,7 +2580,7 @@
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -2559,85 +2588,85 @@
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" s="27"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" s="27"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" s="27"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" s="27"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" s="27"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" s="27"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" s="27"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4">
       <c r="D32" s="27"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="27"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="27"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="27"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="27"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="27"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="27"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="27"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="27"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="27"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="27"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="27"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="27"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="27"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="27"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="27"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="27"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="27"/>
     </row>
   </sheetData>
@@ -2646,16 +2675,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F49"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="33" t="s">
         <v>7</v>
       </c>
@@ -2675,7 +2708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="33">
         <v>1</v>
       </c>
@@ -2695,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="33">
         <v>2</v>
       </c>
@@ -2713,7 +2746,7 @@
       </c>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="33">
         <v>3</v>
       </c>
@@ -2733,7 +2766,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -2753,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="33">
         <v>5</v>
       </c>
@@ -2773,7 +2806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="33">
         <v>6</v>
       </c>
@@ -2786,15 +2819,15 @@
       <c r="D7" s="31">
         <v>41301</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="42" t="s">
         <v>59</v>
       </c>
       <c r="F7" s="32">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="33">
+    <row r="8" spans="1:6">
+      <c r="A8" s="37">
         <v>7</v>
       </c>
       <c r="B8" s="30" t="s">
@@ -2811,11 +2844,11 @@
       </c>
       <c r="F8" s="30"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
+    <row r="9" spans="1:6">
+      <c r="A9" s="37">
         <v>8</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="30" t="s">
@@ -2829,11 +2862,11 @@
       </c>
       <c r="F9" s="30"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="33">
+    <row r="10" spans="1:6">
+      <c r="A10" s="37">
         <v>9</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="30" t="s">
@@ -2849,15 +2882,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="33">
+    <row r="11" spans="1:6">
+      <c r="A11" s="37">
         <v>10</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>13</v>
+      <c r="C11" s="42" t="s">
+        <v>95</v>
       </c>
       <c r="D11" s="31">
         <v>41305</v>
@@ -2869,15 +2902,15 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="33">
+    <row r="12" spans="1:6">
+      <c r="A12" s="37">
         <v>11</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>13</v>
+      <c r="C12" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="D12" s="31">
         <v>41306</v>
@@ -2889,15 +2922,15 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="33">
+    <row r="13" spans="1:6">
+      <c r="A13" s="37">
         <v>12</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>13</v>
+      <c r="C13" s="42" t="s">
+        <v>97</v>
       </c>
       <c r="D13" s="31">
         <v>41306</v>
@@ -2909,15 +2942,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="33">
+    <row r="14" spans="1:6">
+      <c r="A14" s="37">
         <v>13</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>13</v>
+      <c r="C14" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="D14" s="31">
         <v>41307</v>
@@ -2929,105 +2962,169 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
+    <row r="15" spans="1:6">
+      <c r="A15" s="37">
         <v>14</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31">
+      <c r="B15" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="43">
         <v>41308</v>
       </c>
-      <c r="E15" s="30"/>
+      <c r="E15" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="30"/>
+    <row r="16" spans="1:6">
+      <c r="A16" s="37">
+        <v>15</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="43">
+        <v>41309</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="31"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="31"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
+      <c r="A17" s="37">
+        <v>16</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="43">
+        <v>41310</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="37">
+        <v>17</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="43">
+        <v>41311</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="37">
+        <v>18</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="43">
+        <v>41312</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="D28" s="31"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="D29" s="31"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="D31" s="31"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="D32" s="31"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="31"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="31"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="31"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="31"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="31"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="31"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="31"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="31"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="31"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="31"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="31"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="31"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="31"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="31"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="31"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="31"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="31"/>
     </row>
   </sheetData>
@@ -3036,14 +3133,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="11.7109375" style="34"/>
     <col min="4" max="4" width="27.5703125" style="34" customWidth="1"/>
@@ -3051,7 +3148,7 @@
     <col min="6" max="16384" width="11.7109375" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3071,7 +3168,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="21"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -3079,7 +3176,7 @@
       <c r="E2" s="40"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="21"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -3087,7 +3184,7 @@
       <c r="E3" s="40"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="21"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -3095,7 +3192,7 @@
       <c r="E4" s="40"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="21"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -3103,7 +3200,7 @@
       <c r="E5" s="40"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="34" t="s">
         <v>60</v>
       </c>
@@ -3116,7 +3213,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
@@ -3136,7 +3233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="34" t="s">
         <v>60</v>
       </c>
@@ -3150,7 +3247,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
@@ -3170,7 +3267,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="75">
       <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
@@ -3190,7 +3287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="34" t="s">
         <v>60</v>
       </c>
@@ -3210,7 +3307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="34" t="s">
         <v>60</v>
       </c>
@@ -3227,7 +3324,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="34" t="s">
         <v>60</v>
       </c>
@@ -3247,7 +3344,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="34" t="s">
         <v>60</v>
       </c>
@@ -3261,7 +3358,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="34" t="s">
         <v>60</v>
       </c>
@@ -3281,7 +3378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="34" t="s">
         <v>60</v>
       </c>
@@ -3301,7 +3398,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="34" t="s">
         <v>60</v>
       </c>
@@ -3321,7 +3418,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="34" t="s">
         <v>60</v>
       </c>
@@ -3341,7 +3438,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="34" t="s">
         <v>60</v>
       </c>
@@ -3361,7 +3458,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="37" t="s">
         <v>60</v>
       </c>
@@ -3381,7 +3478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30">
       <c r="A21" s="37" t="s">
         <v>60</v>
       </c>
@@ -3401,7 +3498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="37" t="s">
         <v>60</v>
       </c>
@@ -3427,12 +3524,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -3441,7 +3538,7 @@
     <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="45" t="s">
         <v>72</v>
       </c>
@@ -3451,7 +3548,7 @@
       <c r="E1" s="42"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
@@ -3471,7 +3568,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="42" t="s">
         <v>73</v>
       </c>
@@ -3491,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="42" t="s">
         <v>73</v>
       </c>
@@ -3511,7 +3608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="42" t="s">
         <v>73</v>
       </c>
@@ -3531,7 +3628,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="42" t="s">
         <v>73</v>
       </c>
@@ -3551,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45">
       <c r="A7" s="42" t="s">
         <v>73</v>
       </c>
@@ -3571,7 +3668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="42" t="s">
         <v>73</v>
       </c>
@@ -3591,7 +3688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="42" t="s">
         <v>73</v>
       </c>
@@ -3611,7 +3708,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="42" t="s">
         <v>73</v>
       </c>
@@ -3631,7 +3728,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="42" t="s">
         <v>73</v>
       </c>
@@ -3651,7 +3748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="42" t="s">
         <v>73</v>
       </c>
@@ -3671,7 +3768,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="42" t="s">
         <v>73</v>
       </c>
@@ -3691,7 +3788,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="42" t="s">
         <v>73</v>
       </c>
@@ -3711,7 +3808,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="42" t="s">
         <v>73</v>
       </c>
@@ -3731,7 +3828,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3751,7 +3848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="42" t="s">
         <v>73</v>
       </c>
@@ -3771,7 +3868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="42" t="s">
         <v>73</v>
       </c>
@@ -3791,7 +3888,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="42" t="s">
         <v>73</v>
       </c>
@@ -3811,7 +3908,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="42" t="s">
         <v>73</v>
       </c>
@@ -3831,7 +3928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="42" t="s">
         <v>73</v>
       </c>
@@ -3851,7 +3948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="42" t="s">
         <v>73</v>
       </c>
@@ -3871,7 +3968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="42" t="s">
         <v>73</v>
       </c>
@@ -3891,7 +3988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="42" t="s">
         <v>73</v>
       </c>
@@ -3911,7 +4008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="42" t="s">
         <v>73</v>
       </c>
@@ -3931,7 +4028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="42" t="s">
         <v>73</v>
       </c>
@@ -3951,7 +4048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="42" t="s">
         <v>73</v>
       </c>
@@ -3971,7 +4068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="42" t="s">
         <v>73</v>
       </c>
@@ -3991,7 +4088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="42" t="s">
         <v>73</v>
       </c>
@@ -4011,7 +4108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30">
       <c r="A30" s="42" t="s">
         <v>73</v>
       </c>
@@ -4031,7 +4128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="60">
       <c r="A31" s="42" t="s">
         <v>73</v>
       </c>
@@ -4051,7 +4148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="60">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -4071,7 +4168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="42" t="s">
         <v>73</v>
       </c>
@@ -4091,7 +4188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="42" t="s">
         <v>73</v>
       </c>
@@ -4111,7 +4208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="42" t="s">
         <v>73</v>
       </c>
@@ -4131,7 +4228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="42" t="s">
         <v>73</v>
       </c>
@@ -4157,14 +4254,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -4172,7 +4269,7 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
@@ -4192,7 +4289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -4212,7 +4309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -4230,7 +4327,7 @@
       </c>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -4250,7 +4347,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -4270,7 +4367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -4290,7 +4387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -4310,7 +4407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="37">
         <v>7</v>
       </c>
@@ -4328,7 +4425,7 @@
       </c>
       <c r="F8" s="36"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="37">
         <v>8</v>
       </c>
@@ -4346,7 +4443,7 @@
       </c>
       <c r="F9" s="36"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="37">
         <v>9</v>
       </c>
@@ -4366,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="37">
         <v>10</v>
       </c>
@@ -4386,7 +4483,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="37">
         <v>11</v>
       </c>
@@ -4406,7 +4503,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="37">
         <v>12</v>
       </c>
@@ -4426,7 +4523,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="37">
         <v>13</v>
       </c>
@@ -4446,7 +4543,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="37">
         <v>14</v>
       </c>
@@ -4464,7 +4561,7 @@
       </c>
       <c r="F15" s="36"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="37">
         <v>15</v>
       </c>
@@ -4482,7 +4579,7 @@
       </c>
       <c r="F16" s="36"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>16</v>
       </c>
@@ -4500,7 +4597,7 @@
       </c>
       <c r="F17" s="36"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>17</v>
       </c>
@@ -4518,7 +4615,7 @@
       </c>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="37">
         <v>18</v>
       </c>
@@ -4530,7 +4627,7 @@
       <c r="E19" s="34"/>
       <c r="F19" s="36"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="37">
         <v>19</v>
       </c>
@@ -4540,7 +4637,7 @@
       <c r="E20" s="34"/>
       <c r="F20" s="34"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="37">
         <v>20</v>
       </c>
@@ -4550,7 +4647,7 @@
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="37">
         <v>21</v>
       </c>
@@ -4560,7 +4657,7 @@
       <c r="E22" s="34"/>
       <c r="F22" s="34"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="37">
         <v>22</v>
       </c>
@@ -4570,7 +4667,7 @@
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="37">
         <v>23</v>
       </c>
@@ -4580,7 +4677,7 @@
       <c r="E24" s="34"/>
       <c r="F24" s="34"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="37">
         <v>24</v>
       </c>
@@ -4590,7 +4687,7 @@
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="37">
         <v>25</v>
       </c>
@@ -4600,7 +4697,7 @@
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="37">
         <v>26</v>
       </c>
@@ -4610,7 +4707,7 @@
       <c r="E27" s="34"/>
       <c r="F27" s="34"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="37">
         <v>27</v>
       </c>
@@ -4620,7 +4717,7 @@
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="37">
         <v>28</v>
       </c>
@@ -4630,7 +4727,7 @@
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="37">
         <v>29</v>
       </c>
@@ -4640,7 +4737,7 @@
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="37">
         <v>30</v>
       </c>
@@ -4650,7 +4747,7 @@
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="37">
         <v>31</v>
       </c>
@@ -4660,87 +4757,87 @@
       <c r="E32" s="34"/>
       <c r="F32" s="34"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="37">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="37">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="37">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="37">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="37">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="37">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="37">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="37">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="37">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="37">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="37">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="37">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="37">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="37">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="37">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="37">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
updated by sravani date:6/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16485" windowHeight="6390" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16485" windowHeight="6390" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,12 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A7:O25"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="106">
   <si>
     <t>Name</t>
   </si>
@@ -347,6 +346,9 @@
   </si>
   <si>
     <t>coding for student profile</t>
+  </si>
+  <si>
+    <t>KT for team mates</t>
   </si>
 </sst>
 </file>
@@ -2678,7 +2680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -3527,7 +3529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4239,13 +4243,13 @@
         <v>40945</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="46" t="s">
-        <v>18</v>
+        <v>105</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>105</v>
       </c>
       <c r="F36" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Timesheet for Ruchika (MT2012119)
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="13200" windowHeight="4548" firstSheet="1" activeTab="7"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6210" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A15:G20"/>
+  <oleSize ref="A12:G18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -353,6 +353,15 @@
   </si>
   <si>
     <t>Coding for mini project (Student Profile)</t>
+  </si>
+  <si>
+    <t>Nohing</t>
+  </si>
+  <si>
+    <t>Understanding requirement for friend's profile</t>
+  </si>
+  <si>
+    <t>Requirement for Mini Project</t>
   </si>
 </sst>
 </file>
@@ -771,12 +780,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
-    <col min="4" max="4" width="42.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4">
@@ -808,14 +817,14 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1567,14 +1576,14 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1607,7 +1616,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
@@ -2147,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8">
+    <row r="30" spans="1:6" ht="45">
       <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
@@ -2187,7 +2196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="28.8">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="20" t="s">
         <v>15</v>
       </c>
@@ -2227,7 +2236,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2298,7 +2307,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="29" t="s">
@@ -2688,10 +2697,10 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3140,18 +3149,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="11.6640625" style="34"/>
-    <col min="4" max="4" width="27.5546875" style="34" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="11.6640625" style="34"/>
+    <col min="1" max="3" width="11.7109375" style="34"/>
+    <col min="4" max="4" width="27.5703125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="11.7109375" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3219,7 +3228,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
@@ -3253,7 +3262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
@@ -3273,7 +3282,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="72">
+    <row r="10" spans="1:7" ht="75">
       <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
@@ -3293,7 +3302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8">
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="34" t="s">
         <v>60</v>
       </c>
@@ -3313,7 +3322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="34" t="s">
         <v>60</v>
       </c>
@@ -3330,7 +3339,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="34" t="s">
         <v>60</v>
       </c>
@@ -3364,7 +3373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8">
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="34" t="s">
         <v>60</v>
       </c>
@@ -3404,7 +3413,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="34" t="s">
         <v>60</v>
       </c>
@@ -3444,7 +3453,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="34" t="s">
         <v>60</v>
       </c>
@@ -3464,7 +3473,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="37" t="s">
         <v>60</v>
       </c>
@@ -3474,7 +3483,7 @@
       <c r="C20" s="35">
         <v>41308</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="42" t="s">
         <v>62</v>
       </c>
       <c r="E20" s="22" t="s">
@@ -3484,7 +3493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="45">
       <c r="A21" s="37" t="s">
         <v>60</v>
       </c>
@@ -3495,16 +3504,16 @@
         <v>41309</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="F21" s="44">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="37" t="s">
         <v>60</v>
       </c>
@@ -3522,6 +3531,43 @@
       </c>
       <c r="F22" s="44">
         <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="43">
+        <v>41311</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30">
+      <c r="A24" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="43">
+        <v>41312</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="44">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3537,13 +3583,13 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3636,7 +3682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="42" t="s">
         <v>73</v>
       </c>
@@ -3656,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2">
+    <row r="7" spans="1:6" ht="45">
       <c r="A7" s="42" t="s">
         <v>73</v>
       </c>
@@ -3796,7 +3842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.2">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="42" t="s">
         <v>73</v>
       </c>
@@ -3836,7 +3882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8">
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -4116,7 +4162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8">
+    <row r="30" spans="1:6" ht="30">
       <c r="A30" s="42" t="s">
         <v>73</v>
       </c>
@@ -4136,7 +4182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="57.6">
+    <row r="31" spans="1:6" ht="60">
       <c r="A31" s="42" t="s">
         <v>73</v>
       </c>
@@ -4156,7 +4202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="57.6">
+    <row r="32" spans="1:6" ht="60">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -4176,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="42" t="s">
         <v>73</v>
       </c>
@@ -4196,7 +4242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="42" t="s">
         <v>73</v>
       </c>
@@ -4265,16 +4311,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="49.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="2" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
updated by sravani date:7/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6210" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6210" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -366,8 +366,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,7 +563,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -598,7 +597,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -774,14 +772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C5:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -789,7 +787,7 @@
     <col min="4" max="4" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4">
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -797,7 +795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -811,14 +809,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
@@ -828,7 +826,7 @@
     <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
@@ -848,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -868,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -886,7 +884,7 @@
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -906,7 +904,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -926,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -946,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -966,7 +964,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -984,7 +982,7 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -1002,7 +1000,7 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="16">
         <v>9</v>
       </c>
@@ -1022,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -1042,7 +1040,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -1062,7 +1060,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="16">
         <v>12</v>
       </c>
@@ -1082,7 +1080,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="16">
         <v>13</v>
       </c>
@@ -1102,7 +1100,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="16">
         <v>14</v>
       </c>
@@ -1120,7 +1118,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="37">
         <v>15</v>
       </c>
@@ -1138,7 +1136,7 @@
       </c>
       <c r="F16" s="42"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>16</v>
       </c>
@@ -1158,7 +1156,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>17</v>
       </c>
@@ -1178,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="37">
         <v>18</v>
       </c>
@@ -1198,85 +1196,85 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="D49" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="4"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1284,116 +1282,116 @@
       <c r="E53" s="7"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="C54" s="1"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="C56" s="1"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="C59" s="1"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="C60" s="1"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="C61" s="1"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="C63" s="1"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="C64" s="1"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:6">
       <c r="C65" s="1"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:6">
       <c r="C66" s="1"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:6">
       <c r="C67" s="1"/>
       <c r="E67" s="5"/>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6">
       <c r="C68" s="1"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:6">
       <c r="C69" s="1"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:6">
       <c r="C70" s="1"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:6">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:6">
       <c r="C72" s="1"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:6">
       <c r="C73" s="1"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:6">
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:6">
       <c r="C75" s="1"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:6">
       <c r="C76" s="1"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:6">
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:6">
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:6">
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:6">
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="C81" s="1"/>
       <c r="E81" s="5"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="C83" s="1"/>
       <c r="E83" s="5"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="12"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -1401,7 +1399,7 @@
       <c r="E87" s="9"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="12"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -1409,7 +1407,7 @@
       <c r="E88" s="9"/>
       <c r="F88" s="11"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="12"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -1417,7 +1415,7 @@
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="12"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -1425,7 +1423,7 @@
       <c r="E90" s="9"/>
       <c r="F90" s="11"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="12"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -1433,7 +1431,7 @@
       <c r="E91" s="9"/>
       <c r="F91" s="11"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="12"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -1441,7 +1439,7 @@
       <c r="E92" s="9"/>
       <c r="F92" s="11"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="12"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -1449,7 +1447,7 @@
       <c r="E93" s="9"/>
       <c r="F93" s="11"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="12"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -1457,7 +1455,7 @@
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="12"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -1465,7 +1463,7 @@
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="12"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -1473,7 +1471,7 @@
       <c r="E96" s="9"/>
       <c r="F96" s="11"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="12"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -1481,7 +1479,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="11"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="12"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -1489,7 +1487,7 @@
       <c r="E98" s="9"/>
       <c r="F98" s="11"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="12"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -1497,7 +1495,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="11"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="12"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -1505,7 +1503,7 @@
       <c r="E100" s="9"/>
       <c r="F100" s="11"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="12"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -1513,7 +1511,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -1521,66 +1519,66 @@
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103"/>
       <c r="C103" s="1"/>
       <c r="D103" s="10"/>
       <c r="F103" s="6"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104"/>
       <c r="C104" s="1"/>
       <c r="D104" s="10"/>
       <c r="F104" s="6"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105"/>
       <c r="C105" s="1"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:4">
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:4">
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:4">
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:4">
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:4">
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:4">
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:4">
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:4">
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:4">
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:4">
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:4">
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:4">
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:4">
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:4">
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:4">
       <c r="D135" s="10"/>
     </row>
   </sheetData>
@@ -1590,14 +1588,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -1607,7 +1605,7 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -1617,7 +1615,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1635,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1657,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
@@ -1677,7 +1675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="20" t="s">
         <v>15</v>
       </c>
@@ -1697,7 +1695,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="20" t="s">
         <v>15</v>
       </c>
@@ -1717,7 +1715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="20" t="s">
         <v>15</v>
       </c>
@@ -1737,7 +1735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
         <v>15</v>
       </c>
@@ -1757,7 +1755,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="20" t="s">
         <v>15</v>
       </c>
@@ -1777,7 +1775,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="20" t="s">
         <v>15</v>
       </c>
@@ -1797,7 +1795,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="20" t="s">
         <v>15</v>
       </c>
@@ -1817,7 +1815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
@@ -1837,7 +1835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
         <v>15</v>
       </c>
@@ -1857,7 +1855,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="20" t="s">
         <v>15</v>
       </c>
@@ -1877,7 +1875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="20" t="s">
         <v>15</v>
       </c>
@@ -1897,7 +1895,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
@@ -1917,7 +1915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="20" t="s">
         <v>15</v>
       </c>
@@ -1937,7 +1935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="20" t="s">
         <v>15</v>
       </c>
@@ -1957,7 +1955,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="20" t="s">
         <v>15</v>
       </c>
@@ -1977,7 +1975,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="20" t="s">
         <v>15</v>
       </c>
@@ -1997,7 +1995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="20" t="s">
         <v>15</v>
       </c>
@@ -2017,7 +2015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
@@ -2037,7 +2035,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="20" t="s">
         <v>15</v>
       </c>
@@ -2057,7 +2055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="20" t="s">
         <v>15</v>
       </c>
@@ -2077,7 +2075,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="20" t="s">
         <v>15</v>
       </c>
@@ -2097,7 +2095,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="20" t="s">
         <v>15</v>
       </c>
@@ -2117,7 +2115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="20" t="s">
         <v>15</v>
       </c>
@@ -2137,7 +2135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="20" t="s">
         <v>15</v>
       </c>
@@ -2157,7 +2155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="20" t="s">
         <v>15</v>
       </c>
@@ -2177,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="45">
       <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
@@ -2197,7 +2195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="20" t="s">
         <v>15</v>
       </c>
@@ -2217,7 +2215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="20" t="s">
         <v>15</v>
       </c>
@@ -2237,7 +2235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
@@ -2257,7 +2255,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2277,7 +2275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -2297,7 +2295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -2323,14 +2321,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
@@ -2350,7 +2348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="29">
         <v>1</v>
       </c>
@@ -2370,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -2388,7 +2386,7 @@
       </c>
       <c r="F3" s="26"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -2408,7 +2406,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="29">
         <v>4</v>
       </c>
@@ -2428,7 +2426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="29">
         <v>5</v>
       </c>
@@ -2448,7 +2446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="29">
         <v>6</v>
       </c>
@@ -2468,7 +2466,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="29">
         <v>7</v>
       </c>
@@ -2486,7 +2484,7 @@
       </c>
       <c r="F8" s="26"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="29">
         <v>8</v>
       </c>
@@ -2504,7 +2502,7 @@
       </c>
       <c r="F9" s="26"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="29">
         <v>9</v>
       </c>
@@ -2524,7 +2522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="29">
         <v>10</v>
       </c>
@@ -2544,7 +2542,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="29">
         <v>11</v>
       </c>
@@ -2564,7 +2562,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="29">
         <v>12</v>
       </c>
@@ -2584,7 +2582,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="29">
         <v>13</v>
       </c>
@@ -2604,7 +2602,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="29">
         <v>14</v>
       </c>
@@ -2616,7 +2614,7 @@
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -2624,85 +2622,85 @@
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" s="27"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" s="27"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" s="27"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" s="27"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" s="27"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" s="27"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" s="27"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4">
       <c r="D32" s="27"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="27"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="27"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="27"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="27"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="27"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="27"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="27"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="27"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="27"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="27"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="27"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="27"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="27"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="27"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="27"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="27"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="27"/>
     </row>
   </sheetData>
@@ -2711,20 +2709,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="33" t="s">
         <v>7</v>
       </c>
@@ -2744,7 +2742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="33">
         <v>1</v>
       </c>
@@ -2764,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="33">
         <v>2</v>
       </c>
@@ -2782,7 +2780,7 @@
       </c>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="33">
         <v>3</v>
       </c>
@@ -2802,7 +2800,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -2822,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="33">
         <v>5</v>
       </c>
@@ -2842,7 +2840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="33">
         <v>6</v>
       </c>
@@ -2862,7 +2860,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="37">
         <v>7</v>
       </c>
@@ -2880,7 +2878,7 @@
       </c>
       <c r="F8" s="30"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="37">
         <v>8</v>
       </c>
@@ -2898,7 +2896,7 @@
       </c>
       <c r="F9" s="30"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="37">
         <v>9</v>
       </c>
@@ -2918,7 +2916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="37">
         <v>10</v>
       </c>
@@ -2938,7 +2936,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="37">
         <v>11</v>
       </c>
@@ -2958,7 +2956,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="37">
         <v>12</v>
       </c>
@@ -2978,7 +2976,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="37">
         <v>13</v>
       </c>
@@ -2998,7 +2996,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="37">
         <v>14</v>
       </c>
@@ -3016,7 +3014,7 @@
       </c>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="37">
         <v>15</v>
       </c>
@@ -3034,7 +3032,7 @@
       </c>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>16</v>
       </c>
@@ -3051,7 +3049,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>17</v>
       </c>
@@ -3071,7 +3069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="37">
         <v>18</v>
       </c>
@@ -3088,79 +3086,79 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="D28" s="31"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="D29" s="31"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="D31" s="31"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="D32" s="31"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="31"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="31"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="31"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="31"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="31"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="31"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="31"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="31"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="31"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="31"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="31"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="31"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="31"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="31"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="31"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="31"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="31"/>
     </row>
   </sheetData>
@@ -3169,14 +3167,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="11.7109375" style="34"/>
     <col min="4" max="4" width="27.5703125" style="34" customWidth="1"/>
@@ -3184,7 +3182,7 @@
     <col min="6" max="16384" width="11.7109375" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3204,7 +3202,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="21"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -3212,7 +3210,7 @@
       <c r="E2" s="40"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="21"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -3220,7 +3218,7 @@
       <c r="E3" s="40"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="21"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -3228,7 +3226,7 @@
       <c r="E4" s="40"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="21"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -3236,7 +3234,7 @@
       <c r="E5" s="40"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="34" t="s">
         <v>60</v>
       </c>
@@ -3249,7 +3247,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
@@ -3269,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="34" t="s">
         <v>60</v>
       </c>
@@ -3283,7 +3281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
@@ -3303,7 +3301,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="75">
       <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
@@ -3323,7 +3321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="34" t="s">
         <v>60</v>
       </c>
@@ -3343,7 +3341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="34" t="s">
         <v>60</v>
       </c>
@@ -3360,7 +3358,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="34" t="s">
         <v>60</v>
       </c>
@@ -3380,7 +3378,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="34" t="s">
         <v>60</v>
       </c>
@@ -3394,7 +3392,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="34" t="s">
         <v>60</v>
       </c>
@@ -3414,7 +3412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="34" t="s">
         <v>60</v>
       </c>
@@ -3434,7 +3432,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="34" t="s">
         <v>60</v>
       </c>
@@ -3454,7 +3452,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="34" t="s">
         <v>60</v>
       </c>
@@ -3474,7 +3472,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="34" t="s">
         <v>60</v>
       </c>
@@ -3494,7 +3492,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="37" t="s">
         <v>60</v>
       </c>
@@ -3514,7 +3512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="45">
       <c r="A21" s="37" t="s">
         <v>60</v>
       </c>
@@ -3534,7 +3532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="37" t="s">
         <v>60</v>
       </c>
@@ -3554,7 +3552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="37" t="s">
         <v>60</v>
       </c>
@@ -3571,7 +3569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30">
       <c r="A24" s="37" t="s">
         <v>60</v>
       </c>
@@ -3597,14 +3595,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -3613,7 +3611,7 @@
     <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="45" t="s">
         <v>72</v>
       </c>
@@ -3623,7 +3621,7 @@
       <c r="E1" s="42"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
@@ -3643,7 +3641,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="42" t="s">
         <v>73</v>
       </c>
@@ -3663,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="42" t="s">
         <v>73</v>
       </c>
@@ -3683,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="42" t="s">
         <v>73</v>
       </c>
@@ -3703,7 +3701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="42" t="s">
         <v>73</v>
       </c>
@@ -3723,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45">
       <c r="A7" s="42" t="s">
         <v>73</v>
       </c>
@@ -3743,7 +3741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="42" t="s">
         <v>73</v>
       </c>
@@ -3763,7 +3761,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="42" t="s">
         <v>73</v>
       </c>
@@ -3783,7 +3781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="42" t="s">
         <v>73</v>
       </c>
@@ -3803,7 +3801,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="42" t="s">
         <v>73</v>
       </c>
@@ -3823,7 +3821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="42" t="s">
         <v>73</v>
       </c>
@@ -3843,7 +3841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="42" t="s">
         <v>73</v>
       </c>
@@ -3863,7 +3861,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="42" t="s">
         <v>73</v>
       </c>
@@ -3883,7 +3881,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="42" t="s">
         <v>73</v>
       </c>
@@ -3903,7 +3901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="42" t="s">
         <v>73</v>
       </c>
@@ -3923,7 +3921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="42" t="s">
         <v>73</v>
       </c>
@@ -3943,7 +3941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="42" t="s">
         <v>73</v>
       </c>
@@ -3963,7 +3961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="42" t="s">
         <v>73</v>
       </c>
@@ -3983,7 +3981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="42" t="s">
         <v>73</v>
       </c>
@@ -4003,7 +4001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="42" t="s">
         <v>73</v>
       </c>
@@ -4023,7 +4021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="42" t="s">
         <v>73</v>
       </c>
@@ -4043,7 +4041,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="42" t="s">
         <v>73</v>
       </c>
@@ -4063,7 +4061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="42" t="s">
         <v>73</v>
       </c>
@@ -4083,7 +4081,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="42" t="s">
         <v>73</v>
       </c>
@@ -4103,7 +4101,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="42" t="s">
         <v>73</v>
       </c>
@@ -4123,7 +4121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="42" t="s">
         <v>73</v>
       </c>
@@ -4143,7 +4141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="42" t="s">
         <v>73</v>
       </c>
@@ -4163,7 +4161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="42" t="s">
         <v>73</v>
       </c>
@@ -4183,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30">
       <c r="A30" s="42" t="s">
         <v>73</v>
       </c>
@@ -4203,7 +4201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="60">
       <c r="A31" s="42" t="s">
         <v>73</v>
       </c>
@@ -4223,7 +4221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="60">
       <c r="A32" s="42" t="s">
         <v>73</v>
       </c>
@@ -4243,7 +4241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="42" t="s">
         <v>73</v>
       </c>
@@ -4263,7 +4261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="42" t="s">
         <v>73</v>
       </c>
@@ -4283,7 +4281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="42" t="s">
         <v>73</v>
       </c>
@@ -4303,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="42" t="s">
         <v>73</v>
       </c>
@@ -4321,6 +4319,26 @@
       </c>
       <c r="F36" s="44">
         <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30">
+      <c r="A37" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="43">
+        <v>40946</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="44">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4329,14 +4347,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -4344,7 +4362,7 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
@@ -4364,7 +4382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -4384,7 +4402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -4402,7 +4420,7 @@
       </c>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -4422,7 +4440,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -4442,7 +4460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -4462,7 +4480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -4482,7 +4500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="37">
         <v>7</v>
       </c>
@@ -4500,7 +4518,7 @@
       </c>
       <c r="F8" s="36"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="37">
         <v>8</v>
       </c>
@@ -4518,7 +4536,7 @@
       </c>
       <c r="F9" s="36"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="37">
         <v>9</v>
       </c>
@@ -4538,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="37">
         <v>10</v>
       </c>
@@ -4558,7 +4576,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="37">
         <v>11</v>
       </c>
@@ -4578,7 +4596,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="37">
         <v>12</v>
       </c>
@@ -4598,7 +4616,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="37">
         <v>13</v>
       </c>
@@ -4618,7 +4636,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="37">
         <v>14</v>
       </c>
@@ -4636,7 +4654,7 @@
       </c>
       <c r="F15" s="36"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="37">
         <v>15</v>
       </c>
@@ -4654,7 +4672,7 @@
       </c>
       <c r="F16" s="36"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>16</v>
       </c>
@@ -4672,7 +4690,7 @@
       </c>
       <c r="F17" s="36"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>17</v>
       </c>
@@ -4690,7 +4708,7 @@
       </c>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="37">
         <v>18</v>
       </c>
@@ -4708,7 +4726,7 @@
       </c>
       <c r="F19" s="36"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="37">
         <v>19</v>
       </c>
@@ -4718,7 +4736,7 @@
       <c r="E20" s="34"/>
       <c r="F20" s="34"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="37">
         <v>20</v>
       </c>
@@ -4728,7 +4746,7 @@
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="37">
         <v>21</v>
       </c>
@@ -4738,7 +4756,7 @@
       <c r="E22" s="34"/>
       <c r="F22" s="34"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="37">
         <v>22</v>
       </c>
@@ -4748,7 +4766,7 @@
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="37">
         <v>23</v>
       </c>
@@ -4758,7 +4776,7 @@
       <c r="E24" s="34"/>
       <c r="F24" s="34"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="37">
         <v>24</v>
       </c>
@@ -4768,7 +4786,7 @@
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="37">
         <v>25</v>
       </c>
@@ -4778,7 +4796,7 @@
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="37">
         <v>26</v>
       </c>
@@ -4788,7 +4806,7 @@
       <c r="E27" s="34"/>
       <c r="F27" s="34"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="37">
         <v>27</v>
       </c>
@@ -4798,7 +4816,7 @@
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="37">
         <v>28</v>
       </c>
@@ -4808,7 +4826,7 @@
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="37">
         <v>29</v>
       </c>
@@ -4818,7 +4836,7 @@
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="37">
         <v>30</v>
       </c>
@@ -4828,7 +4846,7 @@
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="37">
         <v>31</v>
       </c>
@@ -4838,87 +4856,87 @@
       <c r="E32" s="34"/>
       <c r="F32" s="34"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="37">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="37">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="37">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="37">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="37">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="37">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="37">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="37">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="37">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="37">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="37">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="37">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="37">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="37">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="37">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="37">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
updated by sravani date:8/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14940" windowHeight="3165" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14940" windowHeight="3165" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,12 @@
     <sheet name="Sravani" sheetId="7" r:id="rId7"/>
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A2:K10"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -362,6 +361,16 @@
   </si>
   <si>
     <t>Requirement for Mini Project</t>
+  </si>
+  <si>
+    <t>Meeting with SE TA</t>
+  </si>
+  <si>
+    <t>Rework Test transactions and interaction stories</t>
+  </si>
+  <si>
+    <t>Rework Test transactions and
+ interaction stories for my usecases</t>
   </si>
 </sst>
 </file>
@@ -2713,7 +2722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -3600,9 +3609,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -4343,6 +4352,66 @@
       </c>
       <c r="F37" s="44">
         <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="43">
+        <v>40947</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="43">
+        <v>40947</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="45">
+      <c r="A40" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="43">
+        <v>40947</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="44">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing Timesheet for Ruchik(MT2012119)
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="10515" windowHeight="3540" firstSheet="1" activeTab="4"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11700" windowHeight="6210" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="Sruti" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A14:F23"/>
+  <oleSize ref="A20:G26"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -418,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -466,11 +466,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1118,16 +1114,16 @@
       <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="14">
         <v>41308</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="13"/>
@@ -1136,19 +1132,19 @@
       <c r="A16" s="37">
         <v>15</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="41">
         <v>41309</v>
       </c>
-      <c r="E16" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="42"/>
+      <c r="E16" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="40"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="37">
@@ -1200,7 +1196,7 @@
       <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="41">
         <v>41312</v>
       </c>
       <c r="E19" t="s">
@@ -1220,7 +1216,7 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="41">
         <v>41313</v>
       </c>
       <c r="E20" t="s">
@@ -2704,7 +2700,7 @@
       <c r="B35" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="41">
         <v>41309</v>
       </c>
       <c r="D35" t="s">
@@ -2724,7 +2720,7 @@
       <c r="B36" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="41">
         <v>41310</v>
       </c>
       <c r="D36" t="s">
@@ -2746,7 +2742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2887,7 +2883,7 @@
       <c r="D7" s="31">
         <v>41301</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="40" t="s">
         <v>59</v>
       </c>
       <c r="F7" s="32">
@@ -2916,7 +2912,7 @@
       <c r="A9" s="37">
         <v>8</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="30" t="s">
@@ -2934,7 +2930,7 @@
       <c r="A10" s="37">
         <v>9</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="30" t="s">
@@ -2954,10 +2950,10 @@
       <c r="A11" s="37">
         <v>10</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="40" t="s">
         <v>95</v>
       </c>
       <c r="D11" s="31">
@@ -2974,10 +2970,10 @@
       <c r="A12" s="37">
         <v>11</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="40" t="s">
         <v>96</v>
       </c>
       <c r="D12" s="31">
@@ -2994,10 +2990,10 @@
       <c r="A13" s="37">
         <v>12</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D13" s="31">
@@ -3014,10 +3010,10 @@
       <c r="A14" s="37">
         <v>13</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>98</v>
       </c>
       <c r="D14" s="31">
@@ -3034,16 +3030,16 @@
       <c r="A15" s="37">
         <v>14</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="41">
         <v>41308</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="30"/>
@@ -3052,16 +3048,16 @@
       <c r="A16" s="37">
         <v>15</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="41">
         <v>41309</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="30"/>
@@ -3070,16 +3066,16 @@
       <c r="A17" s="37">
         <v>16</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="41">
         <v>41310</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3087,16 +3083,16 @@
       <c r="A18" s="37">
         <v>17</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="41">
         <v>41311</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="40" t="s">
         <v>104</v>
       </c>
       <c r="F18">
@@ -3107,16 +3103,16 @@
       <c r="A19" s="37">
         <v>18</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="41">
         <v>41312</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="40" t="s">
         <v>104</v>
       </c>
       <c r="F19">
@@ -3127,13 +3123,13 @@
       <c r="A20" s="37">
         <v>19</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="41">
         <v>41313</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="40" t="s">
         <v>104</v>
       </c>
       <c r="F20">
@@ -3222,10 +3218,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
@@ -3237,411 +3233,773 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="47" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="21"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="25"/>
+    <row r="2" spans="1:7" ht="75">
+      <c r="A2" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="41">
+        <v>41278</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="42">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="21"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="25"/>
+      <c r="A3" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="41">
+        <v>41279</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="42">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="21"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="41">
+        <v>41280</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="42">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="21"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="25"/>
+      <c r="A5" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="41">
+        <v>41281</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="42">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="39"/>
+      <c r="C6" s="41">
+        <v>41282</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="42">
+        <v>2</v>
+      </c>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="30">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="41">
+        <v>41283</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="41">
+        <v>41284</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="41">
+        <v>41285</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="41">
+        <v>41286</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="41">
+        <v>41287</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="41">
+        <v>41288</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="41">
+        <v>41289</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="41">
+        <v>41290</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="90">
+      <c r="A15" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="41">
+        <v>41291</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="41">
+        <v>41292</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="41">
+        <v>41293</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="41">
+        <v>41294</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="41">
+        <v>41295</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="41">
         <v>41296</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D20" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E20" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F20" s="42">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="34" t="s">
+    <row r="21" spans="1:6">
+      <c r="A21" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B21" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C21" s="41">
         <v>41297</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="34" t="s">
+      <c r="D21" s="40"/>
+      <c r="E21" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="40"/>
+    </row>
+    <row r="22" spans="1:6" ht="30">
+      <c r="A22" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B22" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C22" s="41">
         <v>41298</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D22" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E22" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F22" s="42">
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75">
-      <c r="A10" s="34" t="s">
+    <row r="23" spans="1:6" ht="75">
+      <c r="A23" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B23" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C23" s="41">
         <v>41299</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D23" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E23" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F23" s="42">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
-      <c r="A11" s="34" t="s">
+    <row r="24" spans="1:6" ht="45">
+      <c r="A24" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B24" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C24" s="41">
         <v>41300</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D24" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E24" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F24" s="42">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
-      <c r="A12" s="34" t="s">
+    <row r="25" spans="1:6" ht="30">
+      <c r="A25" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B25" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C25" s="41">
         <v>41301</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D25" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E25" s="44" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="30">
-      <c r="A13" s="34" t="s">
+      <c r="F25" s="40"/>
+    </row>
+    <row r="26" spans="1:6" ht="30">
+      <c r="A26" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B26" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C26" s="41">
         <v>41302</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D26" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E26" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F26" s="42">
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="34" t="s">
+    <row r="27" spans="1:6">
+      <c r="A27" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B27" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C27" s="41">
         <v>41303</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30">
-      <c r="A15" s="34" t="s">
+      <c r="D27" s="40"/>
+      <c r="E27" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="40"/>
+    </row>
+    <row r="28" spans="1:6" ht="30">
+      <c r="A28" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B28" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C28" s="41">
         <v>41304</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D28" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E28" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F28" s="42">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="34" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B29" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C29" s="41">
         <v>41305</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D29" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E29" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="36">
+      <c r="F29" s="42">
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="34" t="s">
+    <row r="30" spans="1:6" ht="30">
+      <c r="A30" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B30" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C30" s="41">
         <v>41306</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D30" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E30" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="36">
+      <c r="F30" s="42">
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="34" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B31" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C31" s="41">
         <v>41306</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D31" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E31" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F31" s="42">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
-      <c r="A19" s="34" t="s">
+    <row r="32" spans="1:6" ht="30">
+      <c r="A32" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B32" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C32" s="41">
         <v>41307</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D32" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E32" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F32" s="42">
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30">
-      <c r="A20" s="37" t="s">
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B33" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C33" s="41">
         <v>41308</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D33" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E33" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="36">
+      <c r="F33" s="42">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="45">
-      <c r="A21" s="37" t="s">
+    <row r="34" spans="1:6" ht="45">
+      <c r="A34" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B34" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C34" s="41">
         <v>41309</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D34" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E34" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F34" s="42">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30">
-      <c r="A22" s="37" t="s">
+    <row r="35" spans="1:6" ht="30">
+      <c r="A35" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B35" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C35" s="41">
         <v>41310</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D35" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="46" t="s">
+      <c r="E35" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F35" s="42">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="37" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B36" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C36" s="41">
         <v>41311</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D36" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="46" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30">
-      <c r="A24" s="37" t="s">
+      <c r="E36" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="40"/>
+    </row>
+    <row r="37" spans="1:6" ht="30">
+      <c r="A37" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B37" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C37" s="41">
         <v>41312</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D37" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="46" t="s">
+      <c r="E37" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F37" s="42">
         <v>9</v>
       </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="37"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="42"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="37"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="42"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="37"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="42"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="37"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="40"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="37"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3666,792 +4024,792 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="47" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="41">
         <v>40912</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="41">
         <v>40913</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="44">
+      <c r="D4" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="41">
         <v>40914</v>
       </c>
-      <c r="D5" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="47" t="s">
+      <c r="D5" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="41">
         <v>40915</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="41">
         <v>40916</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="42">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="41">
         <v>40917</v>
       </c>
-      <c r="D8" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="47" t="s">
+      <c r="D8" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="41">
         <v>40918</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="47" t="s">
+      <c r="D9" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="41">
         <v>40919</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="47" t="s">
+      <c r="D10" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="41">
         <v>40920</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="42">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="41">
         <v>40921</v>
       </c>
-      <c r="D12" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="47" t="s">
+      <c r="D12" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="41">
         <v>40922</v>
       </c>
-      <c r="D13" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="47" t="s">
+      <c r="D13" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="41">
         <v>40923</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="47" t="s">
+      <c r="F14" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="41">
         <v>40924</v>
       </c>
-      <c r="D15" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="47" t="s">
+      <c r="D15" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="41">
         <v>40925</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="41">
         <v>40926</v>
       </c>
-      <c r="D17" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="47" t="s">
+      <c r="D17" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="41">
         <v>40927</v>
       </c>
-      <c r="D18" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="47" t="s">
+      <c r="D18" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="41">
         <v>40928</v>
       </c>
-      <c r="D19" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="47" t="s">
+      <c r="D19" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="41">
         <v>40929</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="41">
         <v>40930</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="41">
         <v>40931</v>
       </c>
-      <c r="D22" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="47" t="s">
+      <c r="D22" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="41">
         <v>40932</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="44">
+      <c r="F23" s="42">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="41">
         <v>40933</v>
       </c>
-      <c r="D24" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="47" t="s">
+      <c r="D24" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="41">
         <v>40934</v>
       </c>
-      <c r="D25" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="47" t="s">
+      <c r="D25" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="41">
         <v>40935</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="44">
+      <c r="F26" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="41">
         <v>40936</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="44">
+      <c r="F27" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="41">
         <v>40937</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="42" t="s">
+      <c r="E28" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="44">
+      <c r="F28" s="42">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="41">
         <v>40938</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="E29" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F29" s="44">
+      <c r="F29" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="41">
         <v>41305</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="50" t="s">
+      <c r="E30" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="F30" s="44">
+      <c r="F30" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="41">
         <v>40940</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="D31" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="44">
+      <c r="F31" s="42">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="60">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="41">
         <v>40941</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E32" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="44">
+      <c r="F32" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="41">
         <v>40942</v>
       </c>
-      <c r="D33" s="42" t="s">
+      <c r="D33" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="F33" s="44">
+      <c r="F33" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="41">
         <v>40943</v>
       </c>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="46" t="s">
+      <c r="E34" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="F34" s="44">
+      <c r="F34" s="42">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="41">
         <v>40944</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="44">
+      <c r="E35" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="41">
         <v>40945</v>
       </c>
-      <c r="D36" s="42" t="s">
+      <c r="D36" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="44">
+      <c r="F36" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="41">
         <v>40946</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="46" t="s">
+      <c r="E37" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="F37" s="44">
+      <c r="F37" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="30">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="41">
         <v>40947</v>
       </c>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="46" t="s">
+      <c r="E38" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="F38" s="44">
+      <c r="F38" s="42">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="41">
         <v>40947</v>
       </c>
-      <c r="D39" s="42" t="s">
+      <c r="D39" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="F39" s="44">
+      <c r="F39" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="45">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="41">
         <v>40947</v>
       </c>
-      <c r="D40" s="42" t="s">
+      <c r="D40" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="E40" s="46" t="s">
+      <c r="E40" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="F40" s="44">
+      <c r="F40" s="42">
         <v>4</v>
       </c>
     </row>
@@ -4754,16 +5112,16 @@
       <c r="A15" s="37">
         <v>14</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="40" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="35">
         <v>41308</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="40" t="s">
         <v>75</v>
       </c>
       <c r="F15" s="36"/>
@@ -4772,16 +5130,16 @@
       <c r="A16" s="37">
         <v>15</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="35">
         <v>41309</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="40" t="s">
         <v>76</v>
       </c>
       <c r="F16" s="36"/>
@@ -4790,16 +5148,16 @@
       <c r="A17" s="37">
         <v>16</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="40" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="35">
         <v>41310</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="36"/>
@@ -4808,37 +5166,37 @@
       <c r="A18" s="37">
         <v>17</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="40" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="35">
         <v>41311</v>
       </c>
-      <c r="E18" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="44"/>
+      <c r="E18" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="37">
         <v>18</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="40" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="35">
         <v>41312</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="44">
+      <c r="F19" s="42">
         <v>5</v>
       </c>
     </row>
@@ -4846,19 +5204,19 @@
       <c r="A20" s="37">
         <v>19</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="41">
         <v>41313</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="42">
         <v>5</v>
       </c>
     </row>
@@ -4870,7 +5228,7 @@
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
-      <c r="F21" s="44"/>
+      <c r="F21" s="42"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="37">
@@ -4880,7 +5238,7 @@
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
-      <c r="F22" s="44"/>
+      <c r="F22" s="42"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="37">

</xml_diff>